<commit_message>
Mockups de casos de uso 01 y 02
Mockups para los casos de uso de CRU Promoción y Registrar pago de
alumno, se actualiza la plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>Columna</t>
   </si>
@@ -189,6 +189,21 @@
   </si>
   <si>
     <t>Realizar mockup's CU 03 y CU 04</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 01 y CU 02</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 03 y CU 04</t>
+  </si>
+  <si>
+    <t>Realizar mockup de ventana principal de profesor</t>
+  </si>
+  <si>
+    <t>Realizar mockup de ventana principal de director</t>
+  </si>
+  <si>
+    <t>Hecho</t>
   </si>
 </sst>
 </file>
@@ -683,7 +698,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +994,7 @@
         <v>48</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -1008,78 +1023,80 @@
         <v>1</v>
       </c>
       <c r="S6" s="10"/>
-      <c r="T6" s="8"/>
+      <c r="T6" s="8">
+        <v>1</v>
+      </c>
       <c r="U6" s="8">
         <f t="shared" ref="U6:U17" si="3">R6-T6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
         <f t="shared" ref="X6:X17" si="4">U6-W6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
         <f t="shared" ref="AA6:AA17" si="5">X6-Z6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
         <f t="shared" ref="AD6:AD17" si="6">AA6-AC6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
         <f t="shared" ref="AG6:AG17" si="7">AD6-AF6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
         <f t="shared" ref="AJ6:AJ17" si="8">AG6-AI6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
         <f t="shared" ref="AM6:AM17" si="9">AJ6-AL6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
         <f t="shared" ref="AP6:AP17" si="10">AM6-AO6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
         <f t="shared" ref="AS6:AS17" si="11">AP6-AR6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
         <f t="shared" ref="AV6:AV17" si="12">AS6-AU6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
         <f t="shared" ref="AY6:AY17" si="13">AV6-AX6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ6" s="11">
         <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA6" s="11">
         <f t="shared" ref="BA6:BA17" si="15">G6-AZ6</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1092,7 +1109,7 @@
         <v>49</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
@@ -1121,78 +1138,80 @@
         <v>1</v>
       </c>
       <c r="S7" s="10"/>
-      <c r="T7" s="8"/>
+      <c r="T7" s="8">
+        <v>1</v>
+      </c>
       <c r="U7" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V7" s="10"/>
       <c r="W7" s="8"/>
       <c r="X7" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y7" s="10"/>
       <c r="Z7" s="8"/>
       <c r="AA7" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="8"/>
       <c r="AD7" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7" s="10"/>
       <c r="AF7" s="8"/>
       <c r="AG7" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="10"/>
       <c r="AI7" s="8"/>
       <c r="AJ7" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="10"/>
       <c r="AL7" s="8"/>
       <c r="AM7" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN7" s="10"/>
       <c r="AO7" s="8"/>
       <c r="AP7" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="8"/>
       <c r="AS7" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT7" s="10"/>
       <c r="AU7" s="8"/>
       <c r="AV7" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW7" s="10"/>
       <c r="AX7" s="8"/>
       <c r="AY7" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ7" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA7" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -1205,7 +1224,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1234,88 +1253,94 @@
         <v>1</v>
       </c>
       <c r="S8" s="10"/>
-      <c r="T8" s="8"/>
+      <c r="T8" s="8">
+        <v>2</v>
+      </c>
       <c r="U8" s="8">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="V8" s="10"/>
       <c r="W8" s="8"/>
       <c r="X8" s="8">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="Z8" s="8"/>
       <c r="AA8" s="8">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB8" s="10"/>
       <c r="AC8" s="8"/>
       <c r="AD8" s="8">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AE8" s="10"/>
       <c r="AF8" s="8"/>
       <c r="AG8" s="8">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AH8" s="10"/>
       <c r="AI8" s="8"/>
       <c r="AJ8" s="8">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AK8" s="10"/>
       <c r="AL8" s="8"/>
       <c r="AM8" s="8">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AN8" s="10"/>
       <c r="AO8" s="8"/>
       <c r="AP8" s="8">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="8"/>
       <c r="AS8" s="8">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AT8" s="10"/>
       <c r="AU8" s="8"/>
       <c r="AV8" s="8">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AW8" s="10"/>
       <c r="AX8" s="8"/>
       <c r="AY8" s="8">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AZ8" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA8" s="11">
         <f t="shared" si="15"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:53" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G9" s="5"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8">
@@ -1415,16 +1440,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
-        <v>31</v>
-      </c>
+    <row r="10" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G10" s="5"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8">
@@ -1524,14 +1551,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G11" s="5"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8">
@@ -1631,14 +1662,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8">
@@ -2277,6 +2312,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2288,11 +2328,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
descripciones de casos de uso y mockups de ventana principal profesor
Se crean las descripciones de los casos de uso CRU promocion y registrar pago de alumno, tambien el mockup de la pantalla principal del profesor
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Complementos\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -209,7 +209,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -691,14 +691,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA17"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="T8" sqref="T8"/>
+      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,38 +1341,42 @@
       <c r="F9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="8"/>
       <c r="L9" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="8"/>
       <c r="O9" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="10"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" s="10"/>
-      <c r="W9" s="8"/>
+      <c r="W9" s="8">
+        <v>1</v>
+      </c>
       <c r="X9" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1433,7 +1437,7 @@
       </c>
       <c r="AZ9" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA9" s="11">
         <f t="shared" si="15"/>
@@ -1566,35 +1570,36 @@
       <c r="G11" s="5"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="8"/>
       <c r="L11" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="8"/>
       <c r="O11" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="10"/>
       <c r="T11" s="8"/>
       <c r="U11" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="10"/>
-      <c r="W11" s="8"/>
+      <c r="W11" s="8">
+        <v>1</v>
+      </c>
       <c r="X11" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1655,11 +1660,11 @@
       </c>
       <c r="AZ11" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA11" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="2:53" ht="45" x14ac:dyDescent="0.25">
@@ -2312,11 +2317,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2328,6 +2328,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2345,7 +2350,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Descripciones de CU 3 y 4, y ventana principal
Descripciónes para los casos de uso 03 y 04, y mockup de ventana
principal del director.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Complementos\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
   <si>
     <t>Columna</t>
   </si>
@@ -171,9 +171,6 @@
   </si>
   <si>
     <t>Específicar valores de entrada</t>
-  </si>
-  <si>
-    <t>Por iniciar</t>
   </si>
   <si>
     <t>Mario, Vïctor</t>
@@ -209,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -691,11 +688,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="R6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
@@ -991,10 +988,10 @@
         <v>46</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -1103,13 +1100,13 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
@@ -1218,13 +1215,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1333,13 +1330,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
@@ -1448,46 +1445,50 @@
       <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="G10" s="5">
+        <v>1</v>
+      </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="8"/>
       <c r="O10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10" s="10"/>
       <c r="T10" s="8"/>
       <c r="U10" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="10"/>
-      <c r="W10" s="8"/>
+      <c r="W10" s="8">
+        <v>1</v>
+      </c>
       <c r="X10" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1548,7 +1549,7 @@
       </c>
       <c r="AZ10" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA10" s="11">
         <f t="shared" si="15"/>
@@ -1559,15 +1560,17 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8">
         <v>1</v>
@@ -1664,53 +1667,57 @@
       </c>
       <c r="BA11" s="11">
         <f t="shared" si="15"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:53" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="5"/>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="8"/>
       <c r="L12" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="8"/>
       <c r="O12" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="10"/>
       <c r="T12" s="8"/>
       <c r="U12" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="10"/>
-      <c r="W12" s="8"/>
+      <c r="W12" s="8">
+        <v>1</v>
+      </c>
       <c r="X12" s="8">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -1771,7 +1778,7 @@
       </c>
       <c r="AZ12" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA12" s="11">
         <f t="shared" si="15"/>
@@ -2317,6 +2324,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2328,11 +2340,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2350,7 +2357,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Mockups CU 05, 07 y plantilla de tareas
Mockups de los casos de uso de Registrar asistencia y  consulta de
grupos, aparte de actualiza la plantilla de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Instructivo" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$BB$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Casos de Uso'!$A$1:$BB$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
   <si>
     <t>Columna</t>
   </si>
@@ -41,18 +41,6 @@
     <t>Tarea</t>
   </si>
   <si>
-    <t>[Enunciado de tarea 1]</t>
-  </si>
-  <si>
-    <t>[Enunciado de tarea 2]</t>
-  </si>
-  <si>
-    <t>[Enunciado de tarea 3]</t>
-  </si>
-  <si>
-    <t>[Enunciado de tarea 4]</t>
-  </si>
-  <si>
     <t>Estatus</t>
   </si>
   <si>
@@ -125,9 +113,6 @@
     <t>Horas que restan luego de registrarse el consumo diario. Se calcula tomando las horas que restaban el día anterior y se resta las horas consumidas en el día. Si se trata del primer día, se restan las horas del día 1 al estimado de horas totales.</t>
   </si>
   <si>
-    <t>CU-XX</t>
-  </si>
-  <si>
     <t>Identificador (ID) de CU</t>
   </si>
   <si>
@@ -201,6 +186,27 @@
   </si>
   <si>
     <t>Hecho</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 06 y 08</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 05 Y 07</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 09 y 11</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 10 y 12</t>
+  </si>
+  <si>
+    <t>Por iniciar</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 06 y 08</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 05 y 07</t>
   </si>
 </sst>
 </file>
@@ -689,13 +695,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BA17"/>
+  <dimension ref="B1:BA18"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="R6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,7 +764,7 @@
   <sheetData>
     <row r="1" spans="2:53" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="2:53" ht="28.5" x14ac:dyDescent="0.45">
@@ -766,232 +772,232 @@
     </row>
     <row r="3" spans="2:53" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H4" s="14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="9"/>
       <c r="K4" s="14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L4" s="15"/>
       <c r="M4" s="9"/>
       <c r="N4" s="14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O4" s="15"/>
       <c r="P4" s="9"/>
       <c r="Q4" s="14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R4" s="15"/>
       <c r="S4" s="9"/>
       <c r="T4" s="14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="U4" s="15"/>
       <c r="V4" s="9"/>
       <c r="W4" s="14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="X4" s="15"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="AA4" s="15"/>
       <c r="AB4" s="9"/>
       <c r="AC4" s="14" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="AD4" s="15"/>
       <c r="AE4" s="9"/>
       <c r="AF4" s="14" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="AG4" s="15"/>
       <c r="AH4" s="9"/>
       <c r="AI4" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="AJ4" s="15"/>
       <c r="AK4" s="9"/>
       <c r="AL4" s="14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="AM4" s="15"/>
       <c r="AN4" s="9"/>
       <c r="AO4" s="14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="AP4" s="15"/>
       <c r="AQ4" s="9"/>
       <c r="AR4" s="14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="AS4" s="15"/>
       <c r="AT4" s="9"/>
       <c r="AU4" s="14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AV4" s="15"/>
       <c r="AW4" s="9"/>
       <c r="AX4" s="14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="AY4" s="15"/>
       <c r="AZ4" s="14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="BA4" s="15"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="I5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="P5" s="7"/>
       <c r="Q5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="S5" s="7"/>
       <c r="T5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="V5" s="7"/>
       <c r="W5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AB5" s="7"/>
       <c r="AC5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AE5" s="7"/>
       <c r="AF5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AJ5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AK5" s="7"/>
       <c r="AL5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AM5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AN5" s="7"/>
       <c r="AO5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AP5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AQ5" s="7"/>
       <c r="AR5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AT5" s="7"/>
       <c r="AU5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AW5" s="7"/>
       <c r="AX5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AY5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AZ5" s="7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="BA5" s="7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G6" s="5">
         <v>1</v>
@@ -1004,19 +1010,19 @@
       <c r="J6" s="10"/>
       <c r="K6" s="8"/>
       <c r="L6" s="8">
-        <f t="shared" ref="L6:L17" si="0">I6-K6</f>
+        <f t="shared" ref="L6:L18" si="0">I6-K6</f>
         <v>1</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="8"/>
       <c r="O6" s="8">
-        <f t="shared" ref="O6:O17" si="1">L6-N6</f>
+        <f t="shared" ref="O6:O18" si="1">L6-N6</f>
         <v>1</v>
       </c>
       <c r="P6" s="10"/>
       <c r="Q6" s="8"/>
       <c r="R6" s="8">
-        <f t="shared" ref="R6:R17" si="2">O6-Q6</f>
+        <f t="shared" ref="R6:R18" si="2">O6-Q6</f>
         <v>1</v>
       </c>
       <c r="S6" s="10"/>
@@ -1024,75 +1030,75 @@
         <v>1</v>
       </c>
       <c r="U6" s="8">
-        <f t="shared" ref="U6:U17" si="3">R6-T6</f>
+        <f t="shared" ref="U6:U18" si="3">R6-T6</f>
         <v>0</v>
       </c>
       <c r="V6" s="10"/>
       <c r="W6" s="8"/>
       <c r="X6" s="8">
-        <f t="shared" ref="X6:X17" si="4">U6-W6</f>
+        <f t="shared" ref="X6:X18" si="4">U6-W6</f>
         <v>0</v>
       </c>
       <c r="Y6" s="10"/>
       <c r="Z6" s="8"/>
       <c r="AA6" s="8">
-        <f t="shared" ref="AA6:AA17" si="5">X6-Z6</f>
+        <f t="shared" ref="AA6:AA18" si="5">X6-Z6</f>
         <v>0</v>
       </c>
       <c r="AB6" s="10"/>
       <c r="AC6" s="8"/>
       <c r="AD6" s="8">
-        <f t="shared" ref="AD6:AD17" si="6">AA6-AC6</f>
+        <f t="shared" ref="AD6:AD18" si="6">AA6-AC6</f>
         <v>0</v>
       </c>
       <c r="AE6" s="10"/>
       <c r="AF6" s="8"/>
       <c r="AG6" s="8">
-        <f t="shared" ref="AG6:AG17" si="7">AD6-AF6</f>
+        <f t="shared" ref="AG6:AG18" si="7">AD6-AF6</f>
         <v>0</v>
       </c>
       <c r="AH6" s="10"/>
       <c r="AI6" s="8"/>
       <c r="AJ6" s="8">
-        <f t="shared" ref="AJ6:AJ17" si="8">AG6-AI6</f>
+        <f t="shared" ref="AJ6:AJ18" si="8">AG6-AI6</f>
         <v>0</v>
       </c>
       <c r="AK6" s="10"/>
       <c r="AL6" s="8"/>
       <c r="AM6" s="8">
-        <f t="shared" ref="AM6:AM17" si="9">AJ6-AL6</f>
+        <f t="shared" ref="AM6:AM18" si="9">AJ6-AL6</f>
         <v>0</v>
       </c>
       <c r="AN6" s="10"/>
       <c r="AO6" s="8"/>
       <c r="AP6" s="8">
-        <f t="shared" ref="AP6:AP17" si="10">AM6-AO6</f>
+        <f t="shared" ref="AP6:AP18" si="10">AM6-AO6</f>
         <v>0</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="8"/>
       <c r="AS6" s="8">
-        <f t="shared" ref="AS6:AS17" si="11">AP6-AR6</f>
+        <f t="shared" ref="AS6:AS18" si="11">AP6-AR6</f>
         <v>0</v>
       </c>
       <c r="AT6" s="10"/>
       <c r="AU6" s="8"/>
       <c r="AV6" s="8">
-        <f t="shared" ref="AV6:AV17" si="12">AS6-AU6</f>
+        <f t="shared" ref="AV6:AV18" si="12">AS6-AU6</f>
         <v>0</v>
       </c>
       <c r="AW6" s="10"/>
       <c r="AX6" s="8"/>
       <c r="AY6" s="8">
-        <f t="shared" ref="AY6:AY17" si="13">AV6-AX6</f>
+        <f t="shared" ref="AY6:AY18" si="13">AV6-AX6</f>
         <v>0</v>
       </c>
       <c r="AZ6" s="11">
-        <f t="shared" ref="AZ6:AZ16" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
+        <f t="shared" ref="AZ6:AZ17" si="14">H6+K6+N6+Q6+T6+W6+Z6+AC6+AF6+AI6+AL6+AO6+AR6+AU6+AX6</f>
         <v>1</v>
       </c>
       <c r="BA6" s="11">
-        <f t="shared" ref="BA6:BA17" si="15">G6-AZ6</f>
+        <f t="shared" ref="BA6:BA18" si="15">G6-AZ6</f>
         <v>0</v>
       </c>
     </row>
@@ -1100,20 +1106,20 @@
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8">
-        <f t="shared" ref="I7:I17" si="16">G7-H7</f>
+        <f t="shared" ref="I7:I18" si="16">G7-H7</f>
         <v>1</v>
       </c>
       <c r="J7" s="10"/>
@@ -1215,13 +1221,13 @@
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>51</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="G8" s="5">
         <v>1</v>
@@ -1330,13 +1336,13 @@
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G9" s="5">
         <v>1</v>
@@ -1445,13 +1451,13 @@
       <c r="B10" s="13"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -1560,13 +1566,13 @@
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G11" s="5">
         <v>1</v>
@@ -1674,13 +1680,13 @@
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
@@ -1785,230 +1791,248 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+        <v>52</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1</v>
+      </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="8"/>
       <c r="L13" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M13" s="10"/>
       <c r="N13" s="8"/>
       <c r="O13" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="10"/>
       <c r="T13" s="8"/>
       <c r="U13" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="10"/>
       <c r="W13" s="8"/>
       <c r="X13" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="10"/>
-      <c r="Z13" s="8"/>
+      <c r="Z13" s="8">
+        <v>2</v>
+      </c>
       <c r="AA13" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB13" s="10"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE13" s="10"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH13" s="10"/>
       <c r="AI13" s="8"/>
       <c r="AJ13" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK13" s="10"/>
       <c r="AL13" s="8"/>
       <c r="AM13" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN13" s="10"/>
       <c r="AO13" s="8"/>
       <c r="AP13" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT13" s="10"/>
       <c r="AU13" s="8"/>
       <c r="AV13" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW13" s="10"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ13" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA13" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B14" s="13" t="s">
-        <v>31</v>
-      </c>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+        <v>53</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1</v>
+      </c>
       <c r="H14" s="8"/>
       <c r="I14" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="8"/>
       <c r="L14" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="10"/>
       <c r="N14" s="8"/>
       <c r="O14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="10"/>
       <c r="T14" s="8"/>
       <c r="U14" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="10"/>
       <c r="W14" s="8"/>
       <c r="X14" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14" s="10"/>
-      <c r="Z14" s="8"/>
+      <c r="Z14" s="8">
+        <v>2</v>
+      </c>
       <c r="AA14" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB14" s="10"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE14" s="10"/>
       <c r="AF14" s="8"/>
       <c r="AG14" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH14" s="10"/>
       <c r="AI14" s="8"/>
       <c r="AJ14" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK14" s="10"/>
       <c r="AL14" s="8"/>
       <c r="AM14" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN14" s="10"/>
       <c r="AO14" s="8"/>
       <c r="AP14" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT14" s="10"/>
       <c r="AU14" s="8"/>
       <c r="AV14" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW14" s="10"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ14" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA14" s="11">
         <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:53" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G15" s="5"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8">
@@ -2048,7 +2072,7 @@
       <c r="Y15" s="10"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="8">
-        <f t="shared" si="5"/>
+        <f>X15 - Z15</f>
         <v>0</v>
       </c>
       <c r="AB15" s="10"/>
@@ -2099,23 +2123,21 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AZ15" s="11">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="BA15" s="11">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:53" x14ac:dyDescent="0.25">
+      <c r="AZ15" s="11"/>
+      <c r="BA15" s="11"/>
+    </row>
+    <row r="16" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+        <v>55</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G16" s="5"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8">
@@ -2215,14 +2237,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:53" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+        <v>57</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>56</v>
+      </c>
       <c r="G17" s="5"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8">
@@ -2313,11 +2339,122 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AZ17" s="11" t="e">
-        <f>H17+K17+N17+Q17+T17+W17+Z17+AC17+AF17+AI17+AL17+AO17+AR17+AU17+AX17+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+      <c r="AZ17" s="11">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BA17" s="11">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="10"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="10"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S18" s="10"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V18" s="10"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="8"/>
+      <c r="AM18" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AN18" s="10"/>
+      <c r="AO18" s="8"/>
+      <c r="AP18" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AQ18" s="10"/>
+      <c r="AR18" s="8"/>
+      <c r="AS18" s="8">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AT18" s="10"/>
+      <c r="AU18" s="8"/>
+      <c r="AV18" s="8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AW18" s="10"/>
+      <c r="AX18" s="8"/>
+      <c r="AY18" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AZ18" s="11" t="e">
+        <f>H18+K18+N18+Q18+T18+W18+Z18+AC18+AF18+AI18+AL18+AO18+AR18+AU18+AX18+#REF!+#REF!+#REF!+#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="BA17" s="11" t="e">
+      <c r="BA18" s="11" t="e">
         <f t="shared" si="15"/>
         <v>#REF!</v>
       </c>
@@ -2375,12 +2512,12 @@
   <sheetData>
     <row r="1" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B1" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
@@ -2397,7 +2534,7 @@
         <v>Identificador (ID) de CU</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
@@ -2406,7 +2543,7 @@
         <v>Elemento</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="60" x14ac:dyDescent="0.25">
@@ -2414,63 +2551,63 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mockups de CU 10 y 12, y descripciones de 5 y 7
Mockups para los casos de uso de CRU alumno y CRU grupo. Descripciones
de CU 05 Consultar grupos y 07 Registrar asistencia. Se agrega al mockup
de CU 02 - Registrar pago de alumno la opción para marcar si es
incripción o mensualidad. Se actualiza la plantilla de Lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
   <si>
     <t>Columna</t>
   </si>
@@ -207,6 +207,18 @@
   </si>
   <si>
     <t>Realizar descripción de CU 05 y 07</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 14 y 16</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 13 y 15</t>
+  </si>
+  <si>
+    <t>Realizar descripciones de CU  09 y 11</t>
+  </si>
+  <si>
+    <t>Realizar descripciones de CU 10 y 12</t>
   </si>
 </sst>
 </file>
@@ -695,13 +707,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BA18"/>
+  <dimension ref="B1:BA22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2033,95 +2045,99 @@
       <c r="F15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
       <c r="H15" s="8"/>
       <c r="I15" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="10"/>
       <c r="N15" s="8"/>
       <c r="O15" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S15" s="10"/>
       <c r="T15" s="8"/>
       <c r="U15" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15" s="10"/>
       <c r="W15" s="8"/>
       <c r="X15" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y15" s="10"/>
       <c r="Z15" s="8"/>
       <c r="AA15" s="8">
         <f>X15 - Z15</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB15" s="10"/>
-      <c r="AC15" s="8"/>
+      <c r="AC15" s="8">
+        <v>3</v>
+      </c>
       <c r="AD15" s="8">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AE15" s="10"/>
       <c r="AF15" s="8"/>
       <c r="AG15" s="8">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AH15" s="10"/>
       <c r="AI15" s="8"/>
       <c r="AJ15" s="8">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AK15" s="10"/>
       <c r="AL15" s="8"/>
       <c r="AM15" s="8">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AN15" s="10"/>
       <c r="AO15" s="8"/>
       <c r="AP15" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="8">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AT15" s="10"/>
       <c r="AU15" s="8"/>
       <c r="AV15" s="8">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AW15" s="10"/>
       <c r="AX15" s="8"/>
       <c r="AY15" s="8">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AZ15" s="11"/>
       <c r="BA15" s="11"/>
@@ -2136,52 +2152,56 @@
         <v>43</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="G16" s="5">
+        <v>2</v>
+      </c>
       <c r="H16" s="8"/>
       <c r="I16" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="8"/>
       <c r="O16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S16" s="10"/>
       <c r="T16" s="8"/>
       <c r="U16" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V16" s="10"/>
       <c r="W16" s="8"/>
       <c r="X16" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y16" s="10"/>
       <c r="Z16" s="8"/>
       <c r="AA16" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB16" s="10"/>
-      <c r="AC16" s="8"/>
+      <c r="AC16" s="8">
+        <v>2</v>
+      </c>
       <c r="AD16" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2230,7 +2250,7 @@
       </c>
       <c r="AZ16" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BA16" s="11">
         <f t="shared" si="15"/>
@@ -2247,52 +2267,56 @@
         <v>44</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="G17" s="5">
+        <v>1</v>
+      </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="8"/>
       <c r="L17" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="10"/>
       <c r="N17" s="8"/>
       <c r="O17" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="10"/>
       <c r="T17" s="8"/>
       <c r="U17" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="10"/>
       <c r="W17" s="8"/>
       <c r="X17" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="10"/>
       <c r="Z17" s="8"/>
       <c r="AA17" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB17" s="10"/>
-      <c r="AC17" s="8"/>
+      <c r="AC17" s="8">
+        <v>1</v>
+      </c>
       <c r="AD17" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2341,7 +2365,7 @@
       </c>
       <c r="AZ17" s="11">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="11">
         <f t="shared" si="15"/>
@@ -2358,52 +2382,56 @@
         <v>43</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" s="10"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="10"/>
       <c r="T18" s="8"/>
       <c r="U18" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18" s="10"/>
       <c r="W18" s="8"/>
       <c r="X18" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y18" s="10"/>
       <c r="Z18" s="8"/>
       <c r="AA18" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB18" s="10"/>
-      <c r="AC18" s="8"/>
+      <c r="AC18" s="8">
+        <v>1</v>
+      </c>
       <c r="AD18" s="8">
         <f t="shared" si="6"/>
         <v>0</v>
@@ -2456,6 +2484,454 @@
       </c>
       <c r="BA18" s="11" t="e">
         <f t="shared" si="15"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="19" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8">
+        <f t="shared" ref="I19:I22" si="17">G19-H19</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="10"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8">
+        <f t="shared" ref="L19:L22" si="18">I19-K19</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="10"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8">
+        <f t="shared" ref="O19:O22" si="19">L19-N19</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8">
+        <f t="shared" ref="R19:R22" si="20">O19-Q19</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="10"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8">
+        <f t="shared" ref="U19:U22" si="21">R19-T19</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="10"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8">
+        <f t="shared" ref="X19:X22" si="22">U19-W19</f>
+        <v>0</v>
+      </c>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="8"/>
+      <c r="AA19" s="8">
+        <f t="shared" ref="AA19:AA22" si="23">X19-Z19</f>
+        <v>0</v>
+      </c>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="8"/>
+      <c r="AD19" s="8">
+        <f t="shared" ref="AD19:AD22" si="24">AA19-AC19</f>
+        <v>0</v>
+      </c>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="8"/>
+      <c r="AG19" s="8">
+        <f t="shared" ref="AG19:AG22" si="25">AD19-AF19</f>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="8"/>
+      <c r="AJ19" s="8">
+        <f t="shared" ref="AJ19:AJ22" si="26">AG19-AI19</f>
+        <v>0</v>
+      </c>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="8"/>
+      <c r="AM19" s="8">
+        <f t="shared" ref="AM19:AM22" si="27">AJ19-AL19</f>
+        <v>0</v>
+      </c>
+      <c r="AN19" s="10"/>
+      <c r="AO19" s="8"/>
+      <c r="AP19" s="8">
+        <f t="shared" ref="AP19:AP22" si="28">AM19-AO19</f>
+        <v>0</v>
+      </c>
+      <c r="AQ19" s="10"/>
+      <c r="AR19" s="8"/>
+      <c r="AS19" s="8">
+        <f t="shared" ref="AS19:AS22" si="29">AP19-AR19</f>
+        <v>0</v>
+      </c>
+      <c r="AT19" s="10"/>
+      <c r="AU19" s="8"/>
+      <c r="AV19" s="8">
+        <f t="shared" ref="AV19:AV22" si="30">AS19-AU19</f>
+        <v>0</v>
+      </c>
+      <c r="AW19" s="10"/>
+      <c r="AX19" s="8"/>
+      <c r="AY19" s="8">
+        <f t="shared" ref="AY19:AY22" si="31">AV19-AX19</f>
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="11" t="e">
+        <f>H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA19" s="11" t="e">
+        <f t="shared" ref="BA19:BA22" si="32">G19-AZ19</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:53" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="5">
+        <v>2</v>
+      </c>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="J20" s="10"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8">
+        <f t="shared" si="18"/>
+        <v>2</v>
+      </c>
+      <c r="M20" s="10"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8">
+        <f t="shared" si="19"/>
+        <v>2</v>
+      </c>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="S20" s="10"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="V20" s="10"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8">
+        <f t="shared" si="26"/>
+        <v>2</v>
+      </c>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="AQ20" s="10"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="8">
+        <f t="shared" si="29"/>
+        <v>2</v>
+      </c>
+      <c r="AT20" s="10"/>
+      <c r="AU20" s="8"/>
+      <c r="AV20" s="8">
+        <f t="shared" si="30"/>
+        <v>2</v>
+      </c>
+      <c r="AW20" s="10"/>
+      <c r="AX20" s="8"/>
+      <c r="AY20" s="8">
+        <f t="shared" si="31"/>
+        <v>2</v>
+      </c>
+      <c r="AZ20" s="11" t="e">
+        <f>H20+K20+N20+Q20+T20+W20+Z20+AC20+AF20+AI20+AL20+AO20+AR20+AU20+AX20+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA20" s="11" t="e">
+        <f t="shared" si="32"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="10"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="10"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="S21" s="10"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="V21" s="10"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="AN21" s="10"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="AQ21" s="10"/>
+      <c r="AR21" s="8"/>
+      <c r="AS21" s="8">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="AT21" s="10"/>
+      <c r="AU21" s="8"/>
+      <c r="AV21" s="8">
+        <f t="shared" si="30"/>
+        <v>0</v>
+      </c>
+      <c r="AW21" s="10"/>
+      <c r="AX21" s="8"/>
+      <c r="AY21" s="8">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="11" t="e">
+        <f>H21+K21+N21+Q21+T21+W21+Z21+AC21+AF21+AI21+AL21+AO21+AR21+AU21+AX21+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA21" s="11" t="e">
+        <f t="shared" si="32"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="22" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="5">
+        <v>1</v>
+      </c>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="10"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="M22" s="10"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="S22" s="10"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="V22" s="10"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8">
+        <f t="shared" si="25"/>
+        <v>1</v>
+      </c>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="8">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="AN22" s="10"/>
+      <c r="AO22" s="8"/>
+      <c r="AP22" s="8">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="AQ22" s="10"/>
+      <c r="AR22" s="8"/>
+      <c r="AS22" s="8">
+        <f t="shared" si="29"/>
+        <v>1</v>
+      </c>
+      <c r="AT22" s="10"/>
+      <c r="AU22" s="8"/>
+      <c r="AV22" s="8">
+        <f t="shared" si="30"/>
+        <v>1</v>
+      </c>
+      <c r="AW22" s="10"/>
+      <c r="AX22" s="8"/>
+      <c r="AY22" s="8">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="AZ22" s="11" t="e">
+        <f>H22+K22+N22+Q22+T22+W22+Z22+AC22+AF22+AI22+AL22+AO22+AR22+AU22+AX22+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA22" s="11" t="e">
+        <f t="shared" si="32"/>
         <v>#REF!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Mockups de casos de uso 14 y 16,  escripciones de casos de uso 09 y 11.
Se crean los mockups de los casos de uso registrar pago de profesor y registrar gasto promocional asi como las descripciones de los casos de uso consultar alumnos y cambiar alumnos de grupo.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Complementos\plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -224,8 +224,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,8 +256,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +291,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -366,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -402,6 +414,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -706,14 +721,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2499,56 +2514,60 @@
       <c r="F19" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5">
+        <v>1</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8">
         <f t="shared" ref="I19:I22" si="17">G19-H19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8">
         <f t="shared" ref="L19:L22" si="18">I19-K19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8">
         <f t="shared" ref="O19:O22" si="19">L19-N19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8">
         <f t="shared" ref="R19:R22" si="20">O19-Q19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8">
         <f t="shared" ref="U19:U22" si="21">R19-T19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="10"/>
       <c r="W19" s="8"/>
       <c r="X19" s="8">
         <f t="shared" ref="X19:X22" si="22">U19-W19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y19" s="10"/>
       <c r="Z19" s="8"/>
       <c r="AA19" s="8">
         <f t="shared" ref="AA19:AA22" si="23">X19-Z19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB19" s="10"/>
       <c r="AC19" s="8"/>
       <c r="AD19" s="8">
         <f t="shared" ref="AD19:AD22" si="24">AA19-AC19</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE19" s="10"/>
-      <c r="AF19" s="8"/>
+      <c r="AF19" s="8">
+        <v>1</v>
+      </c>
       <c r="AG19" s="8">
         <f t="shared" ref="AG19:AG22" si="25">AD19-AF19</f>
         <v>0</v>
@@ -2723,56 +2742,60 @@
       <c r="F21" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="8"/>
       <c r="X21" s="8">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="8"/>
       <c r="AA21" s="8">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AB21" s="10"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="8">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AE21" s="10"/>
-      <c r="AF21" s="8"/>
+      <c r="AF21" s="16">
+        <v>2</v>
+      </c>
       <c r="AG21" s="8">
         <f t="shared" si="25"/>
         <v>0</v>
@@ -2885,46 +2908,48 @@
         <v>1</v>
       </c>
       <c r="AE22" s="10"/>
-      <c r="AF22" s="8"/>
+      <c r="AF22" s="8">
+        <v>1</v>
+      </c>
       <c r="AG22" s="8">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH22" s="10"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8">
         <f t="shared" si="26"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK22" s="10"/>
       <c r="AL22" s="8"/>
       <c r="AM22" s="8">
         <f t="shared" si="27"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN22" s="10"/>
       <c r="AO22" s="8"/>
       <c r="AP22" s="8">
         <f t="shared" si="28"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ22" s="10"/>
       <c r="AR22" s="8"/>
       <c r="AS22" s="8">
         <f t="shared" si="29"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT22" s="10"/>
       <c r="AU22" s="8"/>
       <c r="AV22" s="8">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW22" s="10"/>
       <c r="AX22" s="8"/>
       <c r="AY22" s="8">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ22" s="11" t="e">
         <f>H22+K22+N22+Q22+T22+W22+Z22+AC22+AF22+AI22+AL22+AO22+AR22+AU22+AX22+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -2937,11 +2962,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2953,6 +2973,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2970,7 +2995,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Mockups CU 13 y 15
Mockups de los CU Consultar historial de pago de profesores y Consultar
todos los grupos, se actualiza la lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -409,14 +409,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -721,14 +721,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA22"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AC24" sqref="AC24"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -803,84 +803,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="15"/>
+      <c r="I4" s="16"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="15"/>
+      <c r="L4" s="16"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="15"/>
+      <c r="O4" s="16"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="15"/>
+      <c r="R4" s="16"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="15"/>
+      <c r="U4" s="16"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="14" t="s">
+      <c r="W4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="15"/>
+      <c r="X4" s="16"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="14" t="s">
+      <c r="Z4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="15"/>
+      <c r="AA4" s="16"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="14" t="s">
+      <c r="AC4" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="15"/>
+      <c r="AD4" s="16"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="14" t="s">
+      <c r="AF4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="15"/>
+      <c r="AG4" s="16"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="14" t="s">
+      <c r="AI4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="15"/>
+      <c r="AJ4" s="16"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="14" t="s">
+      <c r="AL4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="15"/>
+      <c r="AM4" s="16"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="14" t="s">
+      <c r="AO4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="15"/>
+      <c r="AP4" s="16"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="14" t="s">
+      <c r="AR4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="15"/>
+      <c r="AS4" s="16"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="14" t="s">
+      <c r="AU4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="15"/>
+      <c r="AV4" s="16"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="14" t="s">
+      <c r="AX4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="14" t="s">
+      <c r="AY4" s="16"/>
+      <c r="AZ4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="15"/>
+      <c r="BA4" s="16"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -2512,7 +2512,7 @@
         <v>44</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G19" s="5">
         <v>1</v>
@@ -2627,7 +2627,7 @@
         <v>43</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G20" s="5">
         <v>2</v>
@@ -2680,46 +2680,48 @@
         <v>2</v>
       </c>
       <c r="AE20" s="10"/>
-      <c r="AF20" s="8"/>
+      <c r="AF20" s="8">
+        <v>2</v>
+      </c>
       <c r="AG20" s="8">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="10"/>
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8">
         <f t="shared" si="26"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK20" s="10"/>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8">
         <f t="shared" si="27"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN20" s="10"/>
       <c r="AO20" s="8"/>
       <c r="AP20" s="8">
         <f t="shared" si="28"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="8"/>
       <c r="AS20" s="8">
         <f t="shared" si="29"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT20" s="10"/>
       <c r="AU20" s="8"/>
       <c r="AV20" s="8">
         <f t="shared" si="30"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW20" s="10"/>
       <c r="AX20" s="8"/>
       <c r="AY20" s="8">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ20" s="11" t="e">
         <f>H20+K20+N20+Q20+T20+W20+Z20+AC20+AF20+AI20+AL20+AO20+AR20+AU20+AX20+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -2740,7 +2742,7 @@
         <v>44</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G21" s="5">
         <v>2</v>
@@ -2793,7 +2795,7 @@
         <v>2</v>
       </c>
       <c r="AE21" s="10"/>
-      <c r="AF21" s="16">
+      <c r="AF21" s="14">
         <v>2</v>
       </c>
       <c r="AG21" s="8">
@@ -2855,7 +2857,7 @@
         <v>43</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G22" s="5">
         <v>1</v>
@@ -2962,6 +2964,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2973,11 +2980,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2995,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Mockups CU 17 y 19, desccripciones de 13 y 15
Mockups de los CU 17 - Registrar egreso y 19 - CRU Renta espacio,
descripciones de los CU 13 - Consultar historial de pago de profesores y
15 - Consultar todos los grupos, se actualiza la lista de tareas hasta
el día 27 de febrero.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
   <si>
     <t>Columna</t>
   </si>
@@ -219,6 +219,33 @@
   </si>
   <si>
     <t>Realizar descripciones de CU 10 y 12</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 17 y 19</t>
+  </si>
+  <si>
+    <t>Realizar mpckup de CU 20 y 21</t>
+  </si>
+  <si>
+    <t>Realizar descripciones de CU 13 y 15</t>
+  </si>
+  <si>
+    <t>Realizar descripciones de CU 14 y 16</t>
+  </si>
+  <si>
+    <t>En proceso</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU  18 Generar reporte</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 22 - Iniciar sesión</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 17 y 19</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 20 y 21</t>
   </si>
 </sst>
 </file>
@@ -722,13 +749,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BA22"/>
+  <dimension ref="B1:BA30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="K15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2493,13 +2520,13 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AZ18" s="11" t="e">
-        <f>H18+K18+N18+Q18+T18+W18+Z18+AC18+AF18+AI18+AL18+AO18+AR18+AU18+AX18+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA18" s="11" t="e">
+      <c r="AZ18" s="11">
+        <f t="shared" ref="AZ18:AZ25" si="17">H18+K18+N18+Q18+T18+W18+Z18+AC18+AF18+AI18+AL18+AO18+AR18+AU18+AX18</f>
+        <v>1</v>
+      </c>
+      <c r="BA18" s="11">
         <f t="shared" si="15"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2519,49 +2546,49 @@
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8">
-        <f t="shared" ref="I19:I22" si="17">G19-H19</f>
+        <f t="shared" ref="I19:I22" si="18">G19-H19</f>
         <v>1</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8">
-        <f t="shared" ref="L19:L22" si="18">I19-K19</f>
+        <f t="shared" ref="L19:L22" si="19">I19-K19</f>
         <v>1</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8">
-        <f t="shared" ref="O19:O22" si="19">L19-N19</f>
+        <f t="shared" ref="O19:O22" si="20">L19-N19</f>
         <v>1</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8">
-        <f t="shared" ref="R19:R22" si="20">O19-Q19</f>
+        <f t="shared" ref="R19:R22" si="21">O19-Q19</f>
         <v>1</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="8"/>
       <c r="U19" s="8">
-        <f t="shared" ref="U19:U22" si="21">R19-T19</f>
+        <f t="shared" ref="U19:U22" si="22">R19-T19</f>
         <v>1</v>
       </c>
       <c r="V19" s="10"/>
       <c r="W19" s="8"/>
       <c r="X19" s="8">
-        <f t="shared" ref="X19:X22" si="22">U19-W19</f>
+        <f t="shared" ref="X19:X22" si="23">U19-W19</f>
         <v>1</v>
       </c>
       <c r="Y19" s="10"/>
       <c r="Z19" s="8"/>
       <c r="AA19" s="8">
-        <f t="shared" ref="AA19:AA22" si="23">X19-Z19</f>
+        <f t="shared" ref="AA19:AA22" si="24">X19-Z19</f>
         <v>1</v>
       </c>
       <c r="AB19" s="10"/>
       <c r="AC19" s="8"/>
       <c r="AD19" s="8">
-        <f t="shared" ref="AD19:AD22" si="24">AA19-AC19</f>
+        <f t="shared" ref="AD19:AD22" si="25">AA19-AC19</f>
         <v>1</v>
       </c>
       <c r="AE19" s="10"/>
@@ -2569,52 +2596,52 @@
         <v>1</v>
       </c>
       <c r="AG19" s="8">
-        <f t="shared" ref="AG19:AG22" si="25">AD19-AF19</f>
+        <f t="shared" ref="AG19:AG22" si="26">AD19-AF19</f>
         <v>0</v>
       </c>
       <c r="AH19" s="10"/>
       <c r="AI19" s="8"/>
       <c r="AJ19" s="8">
-        <f t="shared" ref="AJ19:AJ22" si="26">AG19-AI19</f>
+        <f t="shared" ref="AJ19:AJ22" si="27">AG19-AI19</f>
         <v>0</v>
       </c>
       <c r="AK19" s="10"/>
       <c r="AL19" s="8"/>
       <c r="AM19" s="8">
-        <f t="shared" ref="AM19:AM22" si="27">AJ19-AL19</f>
+        <f t="shared" ref="AM19:AM22" si="28">AJ19-AL19</f>
         <v>0</v>
       </c>
       <c r="AN19" s="10"/>
       <c r="AO19" s="8"/>
       <c r="AP19" s="8">
-        <f t="shared" ref="AP19:AP22" si="28">AM19-AO19</f>
+        <f t="shared" ref="AP19:AP22" si="29">AM19-AO19</f>
         <v>0</v>
       </c>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="8"/>
       <c r="AS19" s="8">
-        <f t="shared" ref="AS19:AS22" si="29">AP19-AR19</f>
+        <f t="shared" ref="AS19:AS22" si="30">AP19-AR19</f>
         <v>0</v>
       </c>
       <c r="AT19" s="10"/>
       <c r="AU19" s="8"/>
       <c r="AV19" s="8">
-        <f t="shared" ref="AV19:AV22" si="30">AS19-AU19</f>
+        <f t="shared" ref="AV19:AV22" si="31">AS19-AU19</f>
         <v>0</v>
       </c>
       <c r="AW19" s="10"/>
       <c r="AX19" s="8"/>
       <c r="AY19" s="8">
-        <f t="shared" ref="AY19:AY22" si="31">AV19-AX19</f>
-        <v>0</v>
-      </c>
-      <c r="AZ19" s="11" t="e">
-        <f>H19+K19+N19+Q19+T19+W19+Z19+AC19+AF19+AI19+AL19+AO19+AR19+AU19+AX19+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA19" s="11" t="e">
-        <f t="shared" ref="BA19:BA22" si="32">G19-AZ19</f>
-        <v>#REF!</v>
+        <f t="shared" ref="AY19:AY22" si="32">AV19-AX19</f>
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="11">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="BA19" s="11">
+        <f t="shared" ref="BA19:BA22" si="33">G19-AZ19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:53" ht="30" x14ac:dyDescent="0.25">
@@ -2634,49 +2661,49 @@
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="M20" s="10"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="S20" s="10"/>
       <c r="T20" s="8"/>
       <c r="U20" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="V20" s="10"/>
       <c r="W20" s="8"/>
       <c r="X20" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="Y20" s="10"/>
       <c r="Z20" s="8"/>
       <c r="AA20" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="AB20" s="10"/>
       <c r="AC20" s="8"/>
       <c r="AD20" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="AE20" s="10"/>
@@ -2684,52 +2711,52 @@
         <v>2</v>
       </c>
       <c r="AG20" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AH20" s="10"/>
       <c r="AI20" s="8"/>
       <c r="AJ20" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AK20" s="10"/>
       <c r="AL20" s="8"/>
       <c r="AM20" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AN20" s="10"/>
       <c r="AO20" s="8"/>
       <c r="AP20" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="8"/>
       <c r="AS20" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AT20" s="10"/>
       <c r="AU20" s="8"/>
       <c r="AV20" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AW20" s="10"/>
       <c r="AX20" s="8"/>
       <c r="AY20" s="8">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="AZ20" s="11" t="e">
-        <f>H20+K20+N20+Q20+T20+W20+Z20+AC20+AF20+AI20+AL20+AO20+AR20+AU20+AX20+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA20" s="11" t="e">
         <f t="shared" si="32"/>
-        <v>#REF!</v>
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="11">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="BA20" s="11">
+        <f t="shared" si="33"/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:53" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -2749,49 +2776,49 @@
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="8">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>2</v>
       </c>
       <c r="J21" s="10"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>2</v>
       </c>
       <c r="M21" s="10"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="S21" s="10"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>2</v>
       </c>
       <c r="V21" s="10"/>
       <c r="W21" s="8"/>
       <c r="X21" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="Y21" s="10"/>
       <c r="Z21" s="8"/>
       <c r="AA21" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>2</v>
       </c>
       <c r="AB21" s="10"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="AE21" s="10"/>
@@ -2799,52 +2826,52 @@
         <v>2</v>
       </c>
       <c r="AG21" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AH21" s="10"/>
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AK21" s="10"/>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AN21" s="10"/>
       <c r="AO21" s="8"/>
       <c r="AP21" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AQ21" s="10"/>
       <c r="AR21" s="8"/>
       <c r="AS21" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AT21" s="10"/>
       <c r="AU21" s="8"/>
       <c r="AV21" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AW21" s="10"/>
       <c r="AX21" s="8"/>
       <c r="AY21" s="8">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="AZ21" s="11" t="e">
-        <f>H21+K21+N21+Q21+T21+W21+Z21+AC21+AF21+AI21+AL21+AO21+AR21+AU21+AX21+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA21" s="11" t="e">
         <f t="shared" si="32"/>
-        <v>#REF!</v>
+        <v>0</v>
+      </c>
+      <c r="AZ21" s="11">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="BA21" s="11">
+        <f t="shared" si="33"/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2864,49 +2891,49 @@
       </c>
       <c r="H22" s="8"/>
       <c r="I22" s="8">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>1</v>
       </c>
       <c r="M22" s="10"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S22" s="10"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="V22" s="10"/>
       <c r="W22" s="8"/>
       <c r="X22" s="8">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="Y22" s="10"/>
       <c r="Z22" s="8"/>
       <c r="AA22" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="AB22" s="10"/>
       <c r="AC22" s="8"/>
       <c r="AD22" s="8">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="AE22" s="10"/>
@@ -2914,61 +2941,956 @@
         <v>1</v>
       </c>
       <c r="AG22" s="8">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AH22" s="10"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AK22" s="10"/>
       <c r="AL22" s="8"/>
       <c r="AM22" s="8">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AN22" s="10"/>
       <c r="AO22" s="8"/>
       <c r="AP22" s="8">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AQ22" s="10"/>
       <c r="AR22" s="8"/>
       <c r="AS22" s="8">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AT22" s="10"/>
       <c r="AU22" s="8"/>
       <c r="AV22" s="8">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AW22" s="10"/>
       <c r="AX22" s="8"/>
       <c r="AY22" s="8">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="AZ22" s="11" t="e">
-        <f>H22+K22+N22+Q22+T22+W22+Z22+AC22+AF22+AI22+AL22+AO22+AR22+AU22+AX22+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AZ22" s="11">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="BA22" s="11">
+        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G23" s="5">
+        <v>1</v>
+      </c>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8">
+        <f t="shared" ref="I23:I26" si="34">G23-H23</f>
+        <v>1</v>
+      </c>
+      <c r="J23" s="10"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8">
+        <f t="shared" ref="L23:L26" si="35">I23-K23</f>
+        <v>1</v>
+      </c>
+      <c r="M23" s="10"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8">
+        <f t="shared" ref="O23:O26" si="36">L23-N23</f>
+        <v>1</v>
+      </c>
+      <c r="P23" s="10"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8">
+        <f t="shared" ref="R23:R26" si="37">O23-Q23</f>
+        <v>1</v>
+      </c>
+      <c r="S23" s="10"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8">
+        <f t="shared" ref="U23:U26" si="38">R23-T23</f>
+        <v>1</v>
+      </c>
+      <c r="V23" s="10"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8">
+        <f t="shared" ref="X23:X26" si="39">U23-W23</f>
+        <v>1</v>
+      </c>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8">
+        <f t="shared" ref="AA23:AA26" si="40">X23-Z23</f>
+        <v>1</v>
+      </c>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8">
+        <f t="shared" ref="AD23:AD26" si="41">AA23-AC23</f>
+        <v>1</v>
+      </c>
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8">
+        <f t="shared" ref="AG23:AG26" si="42">AD23-AF23</f>
+        <v>1</v>
+      </c>
+      <c r="AH23" s="10"/>
+      <c r="AI23" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ23" s="8">
+        <f t="shared" ref="AJ23:AJ26" si="43">AG23-AI23</f>
+        <v>0</v>
+      </c>
+      <c r="AK23" s="10"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8">
+        <f t="shared" ref="AM23:AM26" si="44">AJ23-AL23</f>
+        <v>0</v>
+      </c>
+      <c r="AN23" s="10"/>
+      <c r="AO23" s="8"/>
+      <c r="AP23" s="8">
+        <f t="shared" ref="AP23:AP26" si="45">AM23-AO23</f>
+        <v>0</v>
+      </c>
+      <c r="AQ23" s="10"/>
+      <c r="AR23" s="8"/>
+      <c r="AS23" s="8">
+        <f t="shared" ref="AS23:AS26" si="46">AP23-AR23</f>
+        <v>0</v>
+      </c>
+      <c r="AT23" s="10"/>
+      <c r="AU23" s="8"/>
+      <c r="AV23" s="8">
+        <f t="shared" ref="AV23:AV26" si="47">AS23-AU23</f>
+        <v>0</v>
+      </c>
+      <c r="AW23" s="10"/>
+      <c r="AX23" s="8"/>
+      <c r="AY23" s="8">
+        <f t="shared" ref="AY23:AY26" si="48">AV23-AX23</f>
+        <v>0</v>
+      </c>
+      <c r="AZ23" s="11">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="BA23" s="11">
+        <f t="shared" ref="BA23:BA26" si="49">G23-AZ23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="10"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="10"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="S24" s="10"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="V24" s="10"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="Y24" s="10"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="10"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="AE24" s="10"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="10"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="AK24" s="10"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="AN24" s="10"/>
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="8">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="10"/>
+      <c r="AR24" s="8"/>
+      <c r="AS24" s="8">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AT24" s="10"/>
+      <c r="AU24" s="8"/>
+      <c r="AV24" s="8">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="AW24" s="10"/>
+      <c r="AX24" s="8"/>
+      <c r="AY24" s="8">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="AZ24" s="11">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BA24" s="11">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8">
+        <f t="shared" si="34"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="10"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+      <c r="M25" s="10"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8">
+        <f t="shared" si="37"/>
+        <v>1</v>
+      </c>
+      <c r="S25" s="10"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8">
+        <f t="shared" si="38"/>
+        <v>1</v>
+      </c>
+      <c r="V25" s="10"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8">
+        <f t="shared" si="39"/>
+        <v>1</v>
+      </c>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="8"/>
+      <c r="AA25" s="8">
+        <f t="shared" si="40"/>
+        <v>1</v>
+      </c>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="8"/>
+      <c r="AD25" s="8">
+        <f t="shared" si="41"/>
+        <v>1</v>
+      </c>
+      <c r="AE25" s="10"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8">
+        <f t="shared" si="42"/>
+        <v>1</v>
+      </c>
+      <c r="AH25" s="10"/>
+      <c r="AI25" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ25" s="8">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="AK25" s="10"/>
+      <c r="AL25" s="8"/>
+      <c r="AM25" s="8">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="AN25" s="10"/>
+      <c r="AO25" s="8"/>
+      <c r="AP25" s="8">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="AQ25" s="10"/>
+      <c r="AR25" s="8"/>
+      <c r="AS25" s="8">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AT25" s="10"/>
+      <c r="AU25" s="8"/>
+      <c r="AV25" s="8">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="AW25" s="10"/>
+      <c r="AX25" s="8"/>
+      <c r="AY25" s="8">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="AZ25" s="11">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="BA25" s="11">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8">
+        <f t="shared" si="34"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="10"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="10"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="S26" s="10"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="V26" s="10"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="8"/>
+      <c r="AA26" s="8">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="8"/>
+      <c r="AD26" s="8">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="10"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="10"/>
+      <c r="AI26" s="8"/>
+      <c r="AJ26" s="8">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="AK26" s="10"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="AN26" s="10"/>
+      <c r="AO26" s="8"/>
+      <c r="AP26" s="8">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="AQ26" s="10"/>
+      <c r="AR26" s="8"/>
+      <c r="AS26" s="8">
+        <f t="shared" si="46"/>
+        <v>0</v>
+      </c>
+      <c r="AT26" s="10"/>
+      <c r="AU26" s="8"/>
+      <c r="AV26" s="8">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="AW26" s="10"/>
+      <c r="AX26" s="8"/>
+      <c r="AY26" s="8">
+        <f t="shared" si="48"/>
+        <v>0</v>
+      </c>
+      <c r="AZ26" s="11" t="e">
+        <f>H26+K26+N26+Q26+T26+W26+Z26+AC26+AF26+AI26+AL26+AO26+AR26+AU26+AX26+#REF!+#REF!+#REF!+#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="BA22" s="11" t="e">
-        <f t="shared" si="32"/>
+      <c r="BA26" s="11" t="e">
+        <f t="shared" si="49"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="27" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="5">
+        <v>2</v>
+      </c>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8">
+        <f t="shared" ref="I27:I30" si="50">G27-H27</f>
+        <v>2</v>
+      </c>
+      <c r="J27" s="10"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8">
+        <f t="shared" ref="L27:L30" si="51">I27-K27</f>
+        <v>2</v>
+      </c>
+      <c r="M27" s="10"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8">
+        <f t="shared" ref="O27:O30" si="52">L27-N27</f>
+        <v>2</v>
+      </c>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="8"/>
+      <c r="R27" s="8">
+        <f t="shared" ref="R27:R30" si="53">O27-Q27</f>
+        <v>2</v>
+      </c>
+      <c r="S27" s="10"/>
+      <c r="T27" s="8"/>
+      <c r="U27" s="8">
+        <f t="shared" ref="U27:U30" si="54">R27-T27</f>
+        <v>2</v>
+      </c>
+      <c r="V27" s="10"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="8">
+        <f t="shared" ref="X27:X30" si="55">U27-W27</f>
+        <v>2</v>
+      </c>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="8"/>
+      <c r="AA27" s="8">
+        <f t="shared" ref="AA27:AA30" si="56">X27-Z27</f>
+        <v>2</v>
+      </c>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="8"/>
+      <c r="AD27" s="8">
+        <f t="shared" ref="AD27:AD30" si="57">AA27-AC27</f>
+        <v>2</v>
+      </c>
+      <c r="AE27" s="10"/>
+      <c r="AF27" s="8"/>
+      <c r="AG27" s="8">
+        <f t="shared" ref="AG27:AG30" si="58">AD27-AF27</f>
+        <v>2</v>
+      </c>
+      <c r="AH27" s="10"/>
+      <c r="AI27" s="8"/>
+      <c r="AJ27" s="8">
+        <f t="shared" ref="AJ27:AJ30" si="59">AG27-AI27</f>
+        <v>2</v>
+      </c>
+      <c r="AK27" s="10"/>
+      <c r="AL27" s="8"/>
+      <c r="AM27" s="8">
+        <f t="shared" ref="AM27:AM30" si="60">AJ27-AL27</f>
+        <v>2</v>
+      </c>
+      <c r="AN27" s="10"/>
+      <c r="AO27" s="8"/>
+      <c r="AP27" s="8">
+        <f t="shared" ref="AP27:AP30" si="61">AM27-AO27</f>
+        <v>2</v>
+      </c>
+      <c r="AQ27" s="10"/>
+      <c r="AR27" s="8"/>
+      <c r="AS27" s="8">
+        <f t="shared" ref="AS27:AS30" si="62">AP27-AR27</f>
+        <v>2</v>
+      </c>
+      <c r="AT27" s="10"/>
+      <c r="AU27" s="8"/>
+      <c r="AV27" s="8">
+        <f t="shared" ref="AV27:AV30" si="63">AS27-AU27</f>
+        <v>2</v>
+      </c>
+      <c r="AW27" s="10"/>
+      <c r="AX27" s="8"/>
+      <c r="AY27" s="8">
+        <f t="shared" ref="AY27:AY30" si="64">AV27-AX27</f>
+        <v>2</v>
+      </c>
+      <c r="AZ27" s="11" t="e">
+        <f>H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA27" s="11" t="e">
+        <f t="shared" ref="BA27:BA30" si="65">G27-AZ27</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="28" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="10"/>
+      <c r="K28" s="8"/>
+      <c r="L28" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="10"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S28" s="10"/>
+      <c r="T28" s="8"/>
+      <c r="U28" s="8">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="V28" s="10"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="10"/>
+      <c r="Z28" s="8"/>
+      <c r="AA28" s="8">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="10"/>
+      <c r="AC28" s="8"/>
+      <c r="AD28" s="8">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="10"/>
+      <c r="AF28" s="8"/>
+      <c r="AG28" s="8">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="AH28" s="10"/>
+      <c r="AI28" s="8"/>
+      <c r="AJ28" s="8">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+      <c r="AK28" s="10"/>
+      <c r="AL28" s="8"/>
+      <c r="AM28" s="8">
+        <f t="shared" si="60"/>
+        <v>0</v>
+      </c>
+      <c r="AN28" s="10"/>
+      <c r="AO28" s="8"/>
+      <c r="AP28" s="8">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="AQ28" s="10"/>
+      <c r="AR28" s="8"/>
+      <c r="AS28" s="8">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="AT28" s="10"/>
+      <c r="AU28" s="8"/>
+      <c r="AV28" s="8">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="AW28" s="10"/>
+      <c r="AX28" s="8"/>
+      <c r="AY28" s="8">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="AZ28" s="11" t="e">
+        <f>H28+K28+N28+Q28+T28+W28+Z28+AC28+AF28+AI28+AL28+AO28+AR28+AU28+AX28+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA28" s="11" t="e">
+        <f t="shared" si="65"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="29" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8">
+        <f t="shared" si="50"/>
+        <v>1</v>
+      </c>
+      <c r="J29" s="10"/>
+      <c r="K29" s="8"/>
+      <c r="L29" s="8">
+        <f t="shared" si="51"/>
+        <v>1</v>
+      </c>
+      <c r="M29" s="10"/>
+      <c r="N29" s="8"/>
+      <c r="O29" s="8">
+        <f t="shared" si="52"/>
+        <v>1</v>
+      </c>
+      <c r="P29" s="10"/>
+      <c r="Q29" s="8"/>
+      <c r="R29" s="8">
+        <f t="shared" si="53"/>
+        <v>1</v>
+      </c>
+      <c r="S29" s="10"/>
+      <c r="T29" s="8"/>
+      <c r="U29" s="8">
+        <f t="shared" si="54"/>
+        <v>1</v>
+      </c>
+      <c r="V29" s="10"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="8">
+        <f t="shared" si="55"/>
+        <v>1</v>
+      </c>
+      <c r="Y29" s="10"/>
+      <c r="Z29" s="8"/>
+      <c r="AA29" s="8">
+        <f t="shared" si="56"/>
+        <v>1</v>
+      </c>
+      <c r="AB29" s="10"/>
+      <c r="AC29" s="8"/>
+      <c r="AD29" s="8">
+        <f t="shared" si="57"/>
+        <v>1</v>
+      </c>
+      <c r="AE29" s="10"/>
+      <c r="AF29" s="8"/>
+      <c r="AG29" s="8">
+        <f t="shared" si="58"/>
+        <v>1</v>
+      </c>
+      <c r="AH29" s="10"/>
+      <c r="AI29" s="8"/>
+      <c r="AJ29" s="8">
+        <f t="shared" si="59"/>
+        <v>1</v>
+      </c>
+      <c r="AK29" s="10"/>
+      <c r="AL29" s="8"/>
+      <c r="AM29" s="8">
+        <f t="shared" si="60"/>
+        <v>1</v>
+      </c>
+      <c r="AN29" s="10"/>
+      <c r="AO29" s="8"/>
+      <c r="AP29" s="8">
+        <f t="shared" si="61"/>
+        <v>1</v>
+      </c>
+      <c r="AQ29" s="10"/>
+      <c r="AR29" s="8"/>
+      <c r="AS29" s="8">
+        <f t="shared" si="62"/>
+        <v>1</v>
+      </c>
+      <c r="AT29" s="10"/>
+      <c r="AU29" s="8"/>
+      <c r="AV29" s="8">
+        <f t="shared" si="63"/>
+        <v>1</v>
+      </c>
+      <c r="AW29" s="10"/>
+      <c r="AX29" s="8"/>
+      <c r="AY29" s="8">
+        <f t="shared" si="64"/>
+        <v>1</v>
+      </c>
+      <c r="AZ29" s="11" t="e">
+        <f>H29+K29+N29+Q29+T29+W29+Z29+AC29+AF29+AI29+AL29+AO29+AR29+AU29+AX29+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA29" s="11" t="e">
+        <f t="shared" si="65"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="30" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="5"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="10"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="8">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="10"/>
+      <c r="N30" s="8"/>
+      <c r="O30" s="8">
+        <f t="shared" si="52"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="8"/>
+      <c r="R30" s="8">
+        <f t="shared" si="53"/>
+        <v>0</v>
+      </c>
+      <c r="S30" s="10"/>
+      <c r="T30" s="8"/>
+      <c r="U30" s="8">
+        <f t="shared" si="54"/>
+        <v>0</v>
+      </c>
+      <c r="V30" s="10"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="8">
+        <f t="shared" si="55"/>
+        <v>0</v>
+      </c>
+      <c r="Y30" s="10"/>
+      <c r="Z30" s="8"/>
+      <c r="AA30" s="8">
+        <f t="shared" si="56"/>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="10"/>
+      <c r="AC30" s="8"/>
+      <c r="AD30" s="8">
+        <f t="shared" si="57"/>
+        <v>0</v>
+      </c>
+      <c r="AE30" s="10"/>
+      <c r="AF30" s="8"/>
+      <c r="AG30" s="8">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+      <c r="AH30" s="10"/>
+      <c r="AI30" s="8"/>
+      <c r="AJ30" s="8">
+        <f t="shared" si="59"/>
+        <v>0</v>
+      </c>
+      <c r="AK30" s="10"/>
+      <c r="AL30" s="8"/>
+      <c r="AM30" s="8">
+        <f t="shared" si="60"/>
+        <v>0</v>
+      </c>
+      <c r="AN30" s="10"/>
+      <c r="AO30" s="8"/>
+      <c r="AP30" s="8">
+        <f t="shared" si="61"/>
+        <v>0</v>
+      </c>
+      <c r="AQ30" s="10"/>
+      <c r="AR30" s="8"/>
+      <c r="AS30" s="8">
+        <f t="shared" si="62"/>
+        <v>0</v>
+      </c>
+      <c r="AT30" s="10"/>
+      <c r="AU30" s="8"/>
+      <c r="AV30" s="8">
+        <f t="shared" si="63"/>
+        <v>0</v>
+      </c>
+      <c r="AW30" s="10"/>
+      <c r="AX30" s="8"/>
+      <c r="AY30" s="8">
+        <f t="shared" si="64"/>
+        <v>0</v>
+      </c>
+      <c r="AZ30" s="11" t="e">
+        <f>H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="BA30" s="11" t="e">
+        <f t="shared" si="65"/>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -2980,6 +3902,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
descripciones de los casos de uso 14 y 16 y mockups de los casos de uso 20 y 21
Se crean las descripciones de los casos de uso registrar pago de profesor y registrar gasto promocional, y mockups de los casos de uso CRU cliente y CRU promoción
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -251,7 +251,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -748,14 +748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
+      <selection pane="bottomRight" activeCell="AI31" sqref="AI31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,62 +3342,66 @@
       <c r="F26" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G26" s="5"/>
+      <c r="G26" s="5">
+        <v>1</v>
+      </c>
       <c r="H26" s="8"/>
       <c r="I26" s="8">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M26" s="10"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="10"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="10"/>
       <c r="W26" s="8"/>
       <c r="X26" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y26" s="10"/>
       <c r="Z26" s="8"/>
       <c r="AA26" s="8">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB26" s="10"/>
       <c r="AC26" s="8"/>
       <c r="AD26" s="8">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE26" s="10"/>
       <c r="AF26" s="8"/>
       <c r="AG26" s="8">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH26" s="10"/>
-      <c r="AI26" s="8"/>
+      <c r="AI26" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ26" s="8">
         <f t="shared" si="43"/>
         <v>0</v>
@@ -3790,62 +3794,66 @@
       <c r="F30" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="G30" s="5"/>
+      <c r="G30" s="5">
+        <v>1</v>
+      </c>
       <c r="H30" s="8"/>
       <c r="I30" s="8">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M30" s="10"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30" s="10"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30" s="10"/>
       <c r="W30" s="8"/>
       <c r="X30" s="8">
         <f t="shared" si="55"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y30" s="10"/>
       <c r="Z30" s="8"/>
       <c r="AA30" s="8">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB30" s="10"/>
       <c r="AC30" s="8"/>
       <c r="AD30" s="8">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE30" s="10"/>
       <c r="AF30" s="8"/>
       <c r="AG30" s="8">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH30" s="10"/>
-      <c r="AI30" s="8"/>
+      <c r="AI30" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ30" s="8">
         <f t="shared" si="59"/>
         <v>0</v>
@@ -3891,6 +3899,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3902,11 +3915,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3924,7 +3932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Mockup CU  18, descripciones CU 17 y 19
Mockup para el CU 18 - Generar reporte de ingresos y egresos,
descripciones de los CU 17 - Registrar egreso y 19 - CRU Renta de
espacio, se actualizan las plantillas de casos de uso y lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -233,25 +233,25 @@
     <t>Realizar descripciones de CU 14 y 16</t>
   </si>
   <si>
+    <t>Realizar mockup de CU  18 Generar reporte</t>
+  </si>
+  <si>
+    <t>Realizar mockup de CU 22 - Iniciar sesión</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 17 y 19</t>
+  </si>
+  <si>
+    <t>Realizar descripción de CU 20 y 21</t>
+  </si>
+  <si>
     <t>En proceso</t>
-  </si>
-  <si>
-    <t>Realizar mockup de CU  18 Generar reporte</t>
-  </si>
-  <si>
-    <t>Realizar mockup de CU 22 - Iniciar sesión</t>
-  </si>
-  <si>
-    <t>Realizar descripción de CU 17 y 19</t>
-  </si>
-  <si>
-    <t>Realizar descripción de CU 20 y 21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -748,14 +748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:BA30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI31" sqref="AI31"/>
+      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,64 +3114,68 @@
         <v>44</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="G24" s="5">
+        <v>1</v>
+      </c>
       <c r="H24" s="8"/>
       <c r="I24" s="8">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8">
         <f t="shared" si="38"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE24" s="10"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
         <f t="shared" si="42"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH24" s="10"/>
-      <c r="AI24" s="8"/>
+      <c r="AI24" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ24" s="8">
         <f t="shared" si="43"/>
         <v>0</v>
@@ -3208,7 +3212,7 @@
       </c>
       <c r="AZ24" s="11">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA24" s="11">
         <f t="shared" si="49"/>
@@ -3340,7 +3344,7 @@
         <v>44</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -3449,13 +3453,13 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G27" s="5">
         <v>2</v>
@@ -3520,34 +3524,36 @@
         <v>2</v>
       </c>
       <c r="AK27" s="10"/>
-      <c r="AL27" s="8"/>
+      <c r="AL27" s="8">
+        <v>2</v>
+      </c>
       <c r="AM27" s="8">
         <f t="shared" ref="AM27:AM30" si="60">AJ27-AL27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AN27" s="10"/>
       <c r="AO27" s="8"/>
       <c r="AP27" s="8">
         <f t="shared" ref="AP27:AP30" si="61">AM27-AO27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AQ27" s="10"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="8">
         <f t="shared" ref="AS27:AS30" si="62">AP27-AR27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AT27" s="10"/>
       <c r="AU27" s="8"/>
       <c r="AV27" s="8">
         <f t="shared" ref="AV27:AV30" si="63">AS27-AU27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AW27" s="10"/>
       <c r="AX27" s="8"/>
       <c r="AY27" s="8">
         <f t="shared" ref="AY27:AY30" si="64">AV27-AX27</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AZ27" s="11" t="e">
         <f>H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -3562,13 +3568,13 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="8"/>
@@ -3673,13 +3679,13 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G29" s="5">
         <v>1</v>
@@ -3744,34 +3750,36 @@
         <v>1</v>
       </c>
       <c r="AK29" s="10"/>
-      <c r="AL29" s="8"/>
+      <c r="AL29" s="8">
+        <v>1</v>
+      </c>
       <c r="AM29" s="8">
         <f t="shared" si="60"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN29" s="10"/>
       <c r="AO29" s="8"/>
       <c r="AP29" s="8">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ29" s="10"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="8">
         <f t="shared" si="62"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT29" s="10"/>
       <c r="AU29" s="8"/>
       <c r="AV29" s="8">
         <f t="shared" si="63"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW29" s="10"/>
       <c r="AX29" s="8"/>
       <c r="AY29" s="8">
         <f t="shared" si="64"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ29" s="11" t="e">
         <f>H29+K29+N29+Q29+T29+W29+Z29+AC29+AF29+AI29+AL29+AO29+AR29+AU29+AX29+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -3786,13 +3794,13 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="G30" s="5">
         <v>1</v>
@@ -3851,42 +3859,40 @@
         <v>1</v>
       </c>
       <c r="AH30" s="10"/>
-      <c r="AI30" s="8">
-        <v>1</v>
-      </c>
+      <c r="AI30" s="8"/>
       <c r="AJ30" s="8">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK30" s="10"/>
       <c r="AL30" s="8"/>
       <c r="AM30" s="8">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="10"/>
       <c r="AO30" s="8"/>
       <c r="AP30" s="8">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ30" s="10"/>
       <c r="AR30" s="8"/>
       <c r="AS30" s="8">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT30" s="10"/>
       <c r="AU30" s="8"/>
       <c r="AV30" s="8">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW30" s="10"/>
       <c r="AX30" s="8"/>
       <c r="AY30" s="8">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ30" s="11" t="e">
         <f>H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -3932,7 +3938,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/Senzho/DesarrolloSoftwareISO"
This reverts commit e90abcc6e6a5f3994a43c3e9efe90e66f13f9ec2, reversing
changes made to 4e91ad56670c3809881820fe55106299246637f2.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Documents\GitHub\DesarrolloSoftwareISO\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de Uso" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">Instructivo!$A$1:$D$15</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Casos de Uso'!$B:$F,'Casos de Uso'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -233,6 +233,9 @@
     <t>Realizar descripciones de CU 14 y 16</t>
   </si>
   <si>
+    <t>En proceso</t>
+  </si>
+  <si>
     <t>Realizar mockup de CU  18 Generar reporte</t>
   </si>
   <si>
@@ -243,15 +246,12 @@
   </si>
   <si>
     <t>Realizar descripción de CU 20 y 21</t>
-  </si>
-  <si>
-    <t>En proceso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -748,14 +748,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BA30"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="H34" sqref="H34"/>
+      <selection pane="bottomRight" activeCell="AI31" sqref="AI31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,68 +3114,64 @@
         <v>44</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G24" s="5">
-        <v>1</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="G24" s="5"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" s="10"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S24" s="10"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V24" s="10"/>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y24" s="10"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB24" s="10"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE24" s="10"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH24" s="10"/>
-      <c r="AI24" s="8">
-        <v>1</v>
-      </c>
+      <c r="AI24" s="8"/>
       <c r="AJ24" s="8">
         <f t="shared" si="43"/>
         <v>0</v>
@@ -3212,7 +3208,7 @@
       </c>
       <c r="AZ24" s="11">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA24" s="11">
         <f t="shared" si="49"/>
@@ -3344,7 +3340,7 @@
         <v>44</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="G26" s="5">
         <v>1</v>
@@ -3453,13 +3449,13 @@
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G27" s="5">
         <v>2</v>
@@ -3524,36 +3520,34 @@
         <v>2</v>
       </c>
       <c r="AK27" s="10"/>
-      <c r="AL27" s="8">
-        <v>2</v>
-      </c>
+      <c r="AL27" s="8"/>
       <c r="AM27" s="8">
         <f t="shared" ref="AM27:AM30" si="60">AJ27-AL27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN27" s="10"/>
       <c r="AO27" s="8"/>
       <c r="AP27" s="8">
         <f t="shared" ref="AP27:AP30" si="61">AM27-AO27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AQ27" s="10"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="8">
         <f t="shared" ref="AS27:AS30" si="62">AP27-AR27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AT27" s="10"/>
       <c r="AU27" s="8"/>
       <c r="AV27" s="8">
         <f t="shared" ref="AV27:AV30" si="63">AS27-AU27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AW27" s="10"/>
       <c r="AX27" s="8"/>
       <c r="AY27" s="8">
         <f t="shared" ref="AY27:AY30" si="64">AV27-AX27</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AZ27" s="11" t="e">
         <f>H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -3568,13 +3562,13 @@
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="8"/>
@@ -3679,13 +3673,13 @@
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>43</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="G29" s="5">
         <v>1</v>
@@ -3750,36 +3744,34 @@
         <v>1</v>
       </c>
       <c r="AK29" s="10"/>
-      <c r="AL29" s="8">
-        <v>1</v>
-      </c>
+      <c r="AL29" s="8"/>
       <c r="AM29" s="8">
         <f t="shared" si="60"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN29" s="10"/>
       <c r="AO29" s="8"/>
       <c r="AP29" s="8">
         <f t="shared" si="61"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ29" s="10"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="8">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT29" s="10"/>
       <c r="AU29" s="8"/>
       <c r="AV29" s="8">
         <f t="shared" si="63"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW29" s="10"/>
       <c r="AX29" s="8"/>
       <c r="AY29" s="8">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ29" s="11" t="e">
         <f>H29+K29+N29+Q29+T29+W29+Z29+AC29+AF29+AI29+AL29+AO29+AR29+AU29+AX29+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -3794,13 +3786,13 @@
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>44</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="G30" s="5">
         <v>1</v>
@@ -3859,40 +3851,42 @@
         <v>1</v>
       </c>
       <c r="AH30" s="10"/>
-      <c r="AI30" s="8"/>
+      <c r="AI30" s="8">
+        <v>1</v>
+      </c>
       <c r="AJ30" s="8">
         <f t="shared" si="59"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK30" s="10"/>
       <c r="AL30" s="8"/>
       <c r="AM30" s="8">
         <f t="shared" si="60"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN30" s="10"/>
       <c r="AO30" s="8"/>
       <c r="AP30" s="8">
         <f t="shared" si="61"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ30" s="10"/>
       <c r="AR30" s="8"/>
       <c r="AS30" s="8">
         <f t="shared" si="62"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT30" s="10"/>
       <c r="AU30" s="8"/>
       <c r="AV30" s="8">
         <f t="shared" si="63"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW30" s="10"/>
       <c r="AX30" s="8"/>
       <c r="AY30" s="8">
         <f t="shared" si="64"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AZ30" s="11" t="e">
         <f>H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30+#REF!+#REF!+#REF!+#REF!+#REF!</f>
@@ -3938,7 +3932,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">

</xml_diff>

<commit_message>
Descripción CU 18 y mockup CU 23
Mockup de CU 23 - Consultar profesores, descripción de CU 18 - Generar
reporte de ingresos y egresos, se actualiza la lista de tareas.
</commit_message>
<xml_diff>
--- a/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
+++ b/Plantillas/Plantilla Lista de Tareas de la Iteración.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Semestre\Tareas y Trabajos\Clon Repo\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Victor Javier\Documents\UV - Ingeniería de Software\6to Semestre\Desarrollo de Software\1er Parcial\Tareas y Trabajos\Clon Repo\Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
   <si>
     <t>Columna</t>
   </si>
@@ -245,7 +245,10 @@
     <t>Realizar descripción de CU 20 y 21</t>
   </si>
   <si>
-    <t>En proceso</t>
+    <t>Descripción de CU 18 y Mockup de CU 23</t>
+  </si>
+  <si>
+    <t>Descripción de CU 22 y mockup de CU 24</t>
   </si>
 </sst>
 </file>
@@ -290,7 +293,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,12 +321,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,14 +433,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -749,13 +746,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:BA30"/>
+  <dimension ref="B1:BA32"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AI29" sqref="AI29"/>
+      <selection pane="bottomRight" activeCell="S37" sqref="S37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,84 +827,84 @@
       </c>
     </row>
     <row r="4" spans="2:53" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="16"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="9"/>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="16"/>
+      <c r="L4" s="15"/>
       <c r="M4" s="9"/>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="16"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="9"/>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="16"/>
+      <c r="R4" s="15"/>
       <c r="S4" s="9"/>
-      <c r="T4" s="15" t="s">
+      <c r="T4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="U4" s="16"/>
+      <c r="U4" s="15"/>
       <c r="V4" s="9"/>
-      <c r="W4" s="15" t="s">
+      <c r="W4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="16"/>
+      <c r="X4" s="15"/>
       <c r="Y4" s="9"/>
-      <c r="Z4" s="15" t="s">
+      <c r="Z4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AA4" s="16"/>
+      <c r="AA4" s="15"/>
       <c r="AB4" s="9"/>
-      <c r="AC4" s="15" t="s">
+      <c r="AC4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AD4" s="16"/>
+      <c r="AD4" s="15"/>
       <c r="AE4" s="9"/>
-      <c r="AF4" s="15" t="s">
+      <c r="AF4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AG4" s="16"/>
+      <c r="AG4" s="15"/>
       <c r="AH4" s="9"/>
-      <c r="AI4" s="15" t="s">
+      <c r="AI4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AJ4" s="16"/>
+      <c r="AJ4" s="15"/>
       <c r="AK4" s="9"/>
-      <c r="AL4" s="15" t="s">
+      <c r="AL4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="AM4" s="16"/>
+      <c r="AM4" s="15"/>
       <c r="AN4" s="9"/>
-      <c r="AO4" s="15" t="s">
+      <c r="AO4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AP4" s="16"/>
+      <c r="AP4" s="15"/>
       <c r="AQ4" s="9"/>
-      <c r="AR4" s="15" t="s">
+      <c r="AR4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="AS4" s="16"/>
+      <c r="AS4" s="15"/>
       <c r="AT4" s="9"/>
-      <c r="AU4" s="15" t="s">
+      <c r="AU4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="AV4" s="16"/>
+      <c r="AV4" s="15"/>
       <c r="AW4" s="9"/>
-      <c r="AX4" s="15" t="s">
+      <c r="AX4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="15" t="s">
+      <c r="AY4" s="15"/>
+      <c r="AZ4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="BA4" s="16"/>
+      <c r="BA4" s="15"/>
     </row>
     <row r="5" spans="2:53" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -2779,97 +2776,97 @@
         <f t="shared" si="18"/>
         <v>2</v>
       </c>
-      <c r="J21" s="10"/>
+      <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8">
         <f t="shared" si="19"/>
         <v>2</v>
       </c>
-      <c r="M21" s="10"/>
+      <c r="M21" s="8"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8">
         <f t="shared" si="20"/>
         <v>2</v>
       </c>
-      <c r="P21" s="10"/>
+      <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="S21" s="10"/>
+      <c r="S21" s="8"/>
       <c r="T21" s="8"/>
       <c r="U21" s="8">
         <f t="shared" si="22"/>
         <v>2</v>
       </c>
-      <c r="V21" s="10"/>
+      <c r="V21" s="8"/>
       <c r="W21" s="8"/>
       <c r="X21" s="8">
         <f t="shared" si="23"/>
         <v>2</v>
       </c>
-      <c r="Y21" s="10"/>
+      <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
       <c r="AA21" s="8">
         <f t="shared" si="24"/>
         <v>2</v>
       </c>
-      <c r="AB21" s="10"/>
+      <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
       <c r="AD21" s="8">
         <f t="shared" si="25"/>
         <v>2</v>
       </c>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="14">
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="16">
         <v>2</v>
       </c>
       <c r="AG21" s="8">
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AH21" s="10"/>
+      <c r="AH21" s="8"/>
       <c r="AI21" s="8"/>
       <c r="AJ21" s="8">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AK21" s="10"/>
+      <c r="AK21" s="8"/>
       <c r="AL21" s="8"/>
       <c r="AM21" s="8">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AN21" s="10"/>
+      <c r="AN21" s="8"/>
       <c r="AO21" s="8"/>
       <c r="AP21" s="8">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AQ21" s="10"/>
+      <c r="AQ21" s="8"/>
       <c r="AR21" s="8"/>
       <c r="AS21" s="8">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AT21" s="10"/>
+      <c r="AT21" s="8"/>
       <c r="AU21" s="8"/>
       <c r="AV21" s="8">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="AW21" s="10"/>
+      <c r="AW21" s="8"/>
       <c r="AX21" s="8"/>
       <c r="AY21" s="8">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AZ21" s="11">
+      <c r="AZ21" s="8">
         <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="BA21" s="11">
+      <c r="BA21" s="8">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -2894,49 +2891,49 @@
         <f t="shared" si="18"/>
         <v>1</v>
       </c>
-      <c r="J22" s="10"/>
+      <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8">
         <f t="shared" si="19"/>
         <v>1</v>
       </c>
-      <c r="M22" s="10"/>
+      <c r="M22" s="8"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8">
         <f t="shared" si="20"/>
         <v>1</v>
       </c>
-      <c r="P22" s="10"/>
+      <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8">
         <f t="shared" si="21"/>
         <v>1</v>
       </c>
-      <c r="S22" s="10"/>
+      <c r="S22" s="8"/>
       <c r="T22" s="8"/>
       <c r="U22" s="8">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="V22" s="10"/>
+      <c r="V22" s="8"/>
       <c r="W22" s="8"/>
       <c r="X22" s="8">
         <f t="shared" si="23"/>
         <v>1</v>
       </c>
-      <c r="Y22" s="10"/>
+      <c r="Y22" s="8"/>
       <c r="Z22" s="8"/>
       <c r="AA22" s="8">
         <f t="shared" si="24"/>
         <v>1</v>
       </c>
-      <c r="AB22" s="10"/>
+      <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
       <c r="AD22" s="8">
         <f t="shared" si="25"/>
         <v>1</v>
       </c>
-      <c r="AE22" s="10"/>
+      <c r="AE22" s="8"/>
       <c r="AF22" s="8">
         <v>1</v>
       </c>
@@ -2944,47 +2941,47 @@
         <f t="shared" si="26"/>
         <v>0</v>
       </c>
-      <c r="AH22" s="10"/>
+      <c r="AH22" s="8"/>
       <c r="AI22" s="8"/>
       <c r="AJ22" s="8">
         <f t="shared" si="27"/>
         <v>0</v>
       </c>
-      <c r="AK22" s="10"/>
+      <c r="AK22" s="8"/>
       <c r="AL22" s="8"/>
       <c r="AM22" s="8">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
-      <c r="AN22" s="10"/>
+      <c r="AN22" s="8"/>
       <c r="AO22" s="8"/>
       <c r="AP22" s="8">
         <f t="shared" si="29"/>
         <v>0</v>
       </c>
-      <c r="AQ22" s="10"/>
+      <c r="AQ22" s="8"/>
       <c r="AR22" s="8"/>
       <c r="AS22" s="8">
         <f t="shared" si="30"/>
         <v>0</v>
       </c>
-      <c r="AT22" s="10"/>
+      <c r="AT22" s="8"/>
       <c r="AU22" s="8"/>
       <c r="AV22" s="8">
         <f t="shared" si="31"/>
         <v>0</v>
       </c>
-      <c r="AW22" s="10"/>
+      <c r="AW22" s="8"/>
       <c r="AX22" s="8"/>
       <c r="AY22" s="8">
         <f t="shared" si="32"/>
         <v>0</v>
       </c>
-      <c r="AZ22" s="11">
+      <c r="AZ22" s="8">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="BA22" s="11">
+      <c r="BA22" s="8">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
@@ -3009,55 +3006,55 @@
         <f t="shared" ref="I23:I26" si="34">G23-H23</f>
         <v>1</v>
       </c>
-      <c r="J23" s="10"/>
+      <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="8">
         <f t="shared" ref="L23:L26" si="35">I23-K23</f>
         <v>1</v>
       </c>
-      <c r="M23" s="10"/>
+      <c r="M23" s="8"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8">
         <f t="shared" ref="O23:O26" si="36">L23-N23</f>
         <v>1</v>
       </c>
-      <c r="P23" s="10"/>
+      <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8">
         <f t="shared" ref="R23:R26" si="37">O23-Q23</f>
         <v>1</v>
       </c>
-      <c r="S23" s="10"/>
+      <c r="S23" s="8"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8">
         <f t="shared" ref="U23:U26" si="38">R23-T23</f>
         <v>1</v>
       </c>
-      <c r="V23" s="10"/>
+      <c r="V23" s="8"/>
       <c r="W23" s="8"/>
       <c r="X23" s="8">
         <f t="shared" ref="X23:X26" si="39">U23-W23</f>
         <v>1</v>
       </c>
-      <c r="Y23" s="10"/>
+      <c r="Y23" s="8"/>
       <c r="Z23" s="8"/>
       <c r="AA23" s="8">
         <f t="shared" ref="AA23:AA26" si="40">X23-Z23</f>
         <v>1</v>
       </c>
-      <c r="AB23" s="10"/>
+      <c r="AB23" s="8"/>
       <c r="AC23" s="8"/>
       <c r="AD23" s="8">
         <f t="shared" ref="AD23:AD26" si="41">AA23-AC23</f>
         <v>1</v>
       </c>
-      <c r="AE23" s="10"/>
+      <c r="AE23" s="8"/>
       <c r="AF23" s="8"/>
       <c r="AG23" s="8">
         <f t="shared" ref="AG23:AG26" si="42">AD23-AF23</f>
         <v>1</v>
       </c>
-      <c r="AH23" s="10"/>
+      <c r="AH23" s="8"/>
       <c r="AI23" s="8">
         <v>1</v>
       </c>
@@ -3065,41 +3062,41 @@
         <f t="shared" ref="AJ23:AJ26" si="43">AG23-AI23</f>
         <v>0</v>
       </c>
-      <c r="AK23" s="10"/>
+      <c r="AK23" s="8"/>
       <c r="AL23" s="8"/>
       <c r="AM23" s="8">
         <f t="shared" ref="AM23:AM26" si="44">AJ23-AL23</f>
         <v>0</v>
       </c>
-      <c r="AN23" s="10"/>
+      <c r="AN23" s="8"/>
       <c r="AO23" s="8"/>
       <c r="AP23" s="8">
         <f t="shared" ref="AP23:AP26" si="45">AM23-AO23</f>
         <v>0</v>
       </c>
-      <c r="AQ23" s="10"/>
+      <c r="AQ23" s="8"/>
       <c r="AR23" s="8"/>
       <c r="AS23" s="8">
         <f t="shared" ref="AS23:AS26" si="46">AP23-AR23</f>
         <v>0</v>
       </c>
-      <c r="AT23" s="10"/>
+      <c r="AT23" s="8"/>
       <c r="AU23" s="8"/>
       <c r="AV23" s="8">
         <f t="shared" ref="AV23:AV26" si="47">AS23-AU23</f>
         <v>0</v>
       </c>
-      <c r="AW23" s="10"/>
+      <c r="AW23" s="8"/>
       <c r="AX23" s="8"/>
       <c r="AY23" s="8">
         <f t="shared" ref="AY23:AY26" si="48">AV23-AX23</f>
         <v>0</v>
       </c>
-      <c r="AZ23" s="11">
+      <c r="AZ23" s="8">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="BA23" s="11">
+      <c r="BA23" s="8">
         <f t="shared" ref="BA23:BA26" si="49">G23-AZ23</f>
         <v>0</v>
       </c>
@@ -3124,55 +3121,55 @@
         <f t="shared" si="34"/>
         <v>1</v>
       </c>
-      <c r="J24" s="10"/>
+      <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="8">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="M24" s="10"/>
+      <c r="M24" s="8"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8">
         <f t="shared" si="36"/>
         <v>1</v>
       </c>
-      <c r="P24" s="10"/>
+      <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
-      <c r="S24" s="10"/>
+      <c r="S24" s="8"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8">
         <f t="shared" si="38"/>
         <v>1</v>
       </c>
-      <c r="V24" s="10"/>
+      <c r="V24" s="8"/>
       <c r="W24" s="8"/>
       <c r="X24" s="8">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="Y24" s="10"/>
+      <c r="Y24" s="8"/>
       <c r="Z24" s="8"/>
       <c r="AA24" s="8">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AB24" s="10"/>
+      <c r="AB24" s="8"/>
       <c r="AC24" s="8"/>
       <c r="AD24" s="8">
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
-      <c r="AE24" s="10"/>
+      <c r="AE24" s="8"/>
       <c r="AF24" s="8"/>
       <c r="AG24" s="8">
         <f t="shared" si="42"/>
         <v>1</v>
       </c>
-      <c r="AH24" s="10"/>
+      <c r="AH24" s="8"/>
       <c r="AI24" s="8">
         <v>1</v>
       </c>
@@ -3180,41 +3177,41 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AK24" s="10"/>
+      <c r="AK24" s="8"/>
       <c r="AL24" s="8"/>
       <c r="AM24" s="8">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AN24" s="10"/>
+      <c r="AN24" s="8"/>
       <c r="AO24" s="8"/>
       <c r="AP24" s="8">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AQ24" s="10"/>
+      <c r="AQ24" s="8"/>
       <c r="AR24" s="8"/>
       <c r="AS24" s="8">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="AT24" s="10"/>
+      <c r="AT24" s="8"/>
       <c r="AU24" s="8"/>
       <c r="AV24" s="8">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="AW24" s="10"/>
+      <c r="AW24" s="8"/>
       <c r="AX24" s="8"/>
       <c r="AY24" s="8">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="AZ24" s="11">
+      <c r="AZ24" s="8">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="BA24" s="11">
+      <c r="BA24" s="8">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
@@ -3239,55 +3236,55 @@
         <f t="shared" si="34"/>
         <v>1</v>
       </c>
-      <c r="J25" s="10"/>
+      <c r="J25" s="8"/>
       <c r="K25" s="8"/>
       <c r="L25" s="8">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="M25" s="10"/>
+      <c r="M25" s="8"/>
       <c r="N25" s="8"/>
       <c r="O25" s="8">
         <f t="shared" si="36"/>
         <v>1</v>
       </c>
-      <c r="P25" s="10"/>
+      <c r="P25" s="8"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
-      <c r="S25" s="10"/>
+      <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8">
         <f t="shared" si="38"/>
         <v>1</v>
       </c>
-      <c r="V25" s="10"/>
+      <c r="V25" s="8"/>
       <c r="W25" s="8"/>
       <c r="X25" s="8">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="Y25" s="10"/>
+      <c r="Y25" s="8"/>
       <c r="Z25" s="8"/>
       <c r="AA25" s="8">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AB25" s="10"/>
+      <c r="AB25" s="8"/>
       <c r="AC25" s="8"/>
       <c r="AD25" s="8">
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
-      <c r="AE25" s="10"/>
+      <c r="AE25" s="8"/>
       <c r="AF25" s="8"/>
       <c r="AG25" s="8">
         <f t="shared" si="42"/>
         <v>1</v>
       </c>
-      <c r="AH25" s="10"/>
+      <c r="AH25" s="8"/>
       <c r="AI25" s="8">
         <v>1</v>
       </c>
@@ -3295,41 +3292,41 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AK25" s="10"/>
+      <c r="AK25" s="8"/>
       <c r="AL25" s="8"/>
       <c r="AM25" s="8">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AN25" s="10"/>
+      <c r="AN25" s="8"/>
       <c r="AO25" s="8"/>
       <c r="AP25" s="8">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AQ25" s="10"/>
+      <c r="AQ25" s="8"/>
       <c r="AR25" s="8"/>
       <c r="AS25" s="8">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="AT25" s="10"/>
+      <c r="AT25" s="8"/>
       <c r="AU25" s="8"/>
       <c r="AV25" s="8">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="AW25" s="10"/>
+      <c r="AW25" s="8"/>
       <c r="AX25" s="8"/>
       <c r="AY25" s="8">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="AZ25" s="11">
+      <c r="AZ25" s="8">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="BA25" s="11">
+      <c r="BA25" s="8">
         <f t="shared" si="49"/>
         <v>0</v>
       </c>
@@ -3354,55 +3351,55 @@
         <f t="shared" si="34"/>
         <v>1</v>
       </c>
-      <c r="J26" s="10"/>
+      <c r="J26" s="8"/>
       <c r="K26" s="8"/>
       <c r="L26" s="8">
         <f t="shared" si="35"/>
         <v>1</v>
       </c>
-      <c r="M26" s="10"/>
+      <c r="M26" s="8"/>
       <c r="N26" s="8"/>
       <c r="O26" s="8">
         <f t="shared" si="36"/>
         <v>1</v>
       </c>
-      <c r="P26" s="10"/>
+      <c r="P26" s="8"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8">
         <f t="shared" si="37"/>
         <v>1</v>
       </c>
-      <c r="S26" s="10"/>
+      <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8">
         <f t="shared" si="38"/>
         <v>1</v>
       </c>
-      <c r="V26" s="10"/>
+      <c r="V26" s="8"/>
       <c r="W26" s="8"/>
       <c r="X26" s="8">
         <f t="shared" si="39"/>
         <v>1</v>
       </c>
-      <c r="Y26" s="10"/>
+      <c r="Y26" s="8"/>
       <c r="Z26" s="8"/>
       <c r="AA26" s="8">
         <f t="shared" si="40"/>
         <v>1</v>
       </c>
-      <c r="AB26" s="10"/>
+      <c r="AB26" s="8"/>
       <c r="AC26" s="8"/>
       <c r="AD26" s="8">
         <f t="shared" si="41"/>
         <v>1</v>
       </c>
-      <c r="AE26" s="10"/>
+      <c r="AE26" s="8"/>
       <c r="AF26" s="8"/>
       <c r="AG26" s="8">
         <f t="shared" si="42"/>
         <v>1</v>
       </c>
-      <c r="AH26" s="10"/>
+      <c r="AH26" s="8"/>
       <c r="AI26" s="8">
         <v>1</v>
       </c>
@@ -3410,43 +3407,43 @@
         <f t="shared" si="43"/>
         <v>0</v>
       </c>
-      <c r="AK26" s="10"/>
+      <c r="AK26" s="8"/>
       <c r="AL26" s="8"/>
       <c r="AM26" s="8">
         <f t="shared" si="44"/>
         <v>0</v>
       </c>
-      <c r="AN26" s="10"/>
+      <c r="AN26" s="8"/>
       <c r="AO26" s="8"/>
       <c r="AP26" s="8">
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="AQ26" s="10"/>
+      <c r="AQ26" s="8"/>
       <c r="AR26" s="8"/>
       <c r="AS26" s="8">
         <f t="shared" si="46"/>
         <v>0</v>
       </c>
-      <c r="AT26" s="10"/>
+      <c r="AT26" s="8"/>
       <c r="AU26" s="8"/>
       <c r="AV26" s="8">
         <f t="shared" si="47"/>
         <v>0</v>
       </c>
-      <c r="AW26" s="10"/>
+      <c r="AW26" s="8"/>
       <c r="AX26" s="8"/>
       <c r="AY26" s="8">
         <f t="shared" si="48"/>
         <v>0</v>
       </c>
-      <c r="AZ26" s="11" t="e">
-        <f>H26+K26+N26+Q26+T26+W26+Z26+AC26+AF26+AI26+AL26+AO26+AR26+AU26+AX26+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA26" s="11" t="e">
+      <c r="AZ26" s="8">
+        <f>H26+K26+N26+Q26+T26+W26+Z26+AC26+AF26+AI26+AL26+AO26+AR26+AU26+AX26</f>
+        <v>1</v>
+      </c>
+      <c r="BA26" s="8">
         <f t="shared" si="49"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3469,61 +3466,61 @@
         <f t="shared" ref="I27:I30" si="50">G27-H27</f>
         <v>2</v>
       </c>
-      <c r="J27" s="10"/>
+      <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8">
         <f t="shared" ref="L27:L30" si="51">I27-K27</f>
         <v>2</v>
       </c>
-      <c r="M27" s="10"/>
+      <c r="M27" s="8"/>
       <c r="N27" s="8"/>
       <c r="O27" s="8">
         <f t="shared" ref="O27:O30" si="52">L27-N27</f>
         <v>2</v>
       </c>
-      <c r="P27" s="10"/>
+      <c r="P27" s="8"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8">
         <f t="shared" ref="R27:R30" si="53">O27-Q27</f>
         <v>2</v>
       </c>
-      <c r="S27" s="10"/>
+      <c r="S27" s="8"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8">
         <f t="shared" ref="U27:U30" si="54">R27-T27</f>
         <v>2</v>
       </c>
-      <c r="V27" s="10"/>
+      <c r="V27" s="8"/>
       <c r="W27" s="8"/>
       <c r="X27" s="8">
         <f t="shared" ref="X27:X30" si="55">U27-W27</f>
         <v>2</v>
       </c>
-      <c r="Y27" s="10"/>
+      <c r="Y27" s="8"/>
       <c r="Z27" s="8"/>
       <c r="AA27" s="8">
         <f t="shared" ref="AA27:AA30" si="56">X27-Z27</f>
         <v>2</v>
       </c>
-      <c r="AB27" s="10"/>
+      <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
       <c r="AD27" s="8">
         <f t="shared" ref="AD27:AD30" si="57">AA27-AC27</f>
         <v>2</v>
       </c>
-      <c r="AE27" s="10"/>
+      <c r="AE27" s="8"/>
       <c r="AF27" s="8"/>
       <c r="AG27" s="8">
         <f t="shared" ref="AG27:AG30" si="58">AD27-AF27</f>
         <v>2</v>
       </c>
-      <c r="AH27" s="10"/>
+      <c r="AH27" s="8"/>
       <c r="AI27" s="8"/>
       <c r="AJ27" s="8">
         <f t="shared" ref="AJ27:AJ30" si="59">AG27-AI27</f>
         <v>2</v>
       </c>
-      <c r="AK27" s="10"/>
+      <c r="AK27" s="8"/>
       <c r="AL27" s="8">
         <v>2</v>
       </c>
@@ -3531,37 +3528,37 @@
         <f t="shared" ref="AM27:AM30" si="60">AJ27-AL27</f>
         <v>0</v>
       </c>
-      <c r="AN27" s="10"/>
+      <c r="AN27" s="8"/>
       <c r="AO27" s="8"/>
       <c r="AP27" s="8">
         <f t="shared" ref="AP27:AP30" si="61">AM27-AO27</f>
         <v>0</v>
       </c>
-      <c r="AQ27" s="10"/>
+      <c r="AQ27" s="8"/>
       <c r="AR27" s="8"/>
       <c r="AS27" s="8">
         <f t="shared" ref="AS27:AS30" si="62">AP27-AR27</f>
         <v>0</v>
       </c>
-      <c r="AT27" s="10"/>
+      <c r="AT27" s="8"/>
       <c r="AU27" s="8"/>
       <c r="AV27" s="8">
         <f t="shared" ref="AV27:AV30" si="63">AS27-AU27</f>
         <v>0</v>
       </c>
-      <c r="AW27" s="10"/>
+      <c r="AW27" s="8"/>
       <c r="AX27" s="8"/>
       <c r="AY27" s="8">
         <f t="shared" ref="AY27:AY30" si="64">AV27-AX27</f>
         <v>0</v>
       </c>
-      <c r="AZ27" s="11" t="e">
-        <f>H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA27" s="11" t="e">
+      <c r="AZ27" s="8">
+        <f>H27+K27+N27+Q27+T27+W27+Z27+AC27+AF27+AI27+AL27+AO27+AR27+AU27+AX27</f>
+        <v>2</v>
+      </c>
+      <c r="BA27" s="8">
         <f t="shared" ref="BA27:BA30" si="65">G27-AZ27</f>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3584,61 +3581,61 @@
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
-      <c r="J28" s="10"/>
+      <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8">
         <f t="shared" si="51"/>
         <v>1</v>
       </c>
-      <c r="M28" s="10"/>
+      <c r="M28" s="8"/>
       <c r="N28" s="8"/>
       <c r="O28" s="8">
         <f t="shared" si="52"/>
         <v>1</v>
       </c>
-      <c r="P28" s="10"/>
+      <c r="P28" s="8"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
-      <c r="S28" s="10"/>
+      <c r="S28" s="8"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8">
         <f t="shared" si="54"/>
         <v>1</v>
       </c>
-      <c r="V28" s="10"/>
+      <c r="V28" s="8"/>
       <c r="W28" s="8"/>
       <c r="X28" s="8">
         <f t="shared" si="55"/>
         <v>1</v>
       </c>
-      <c r="Y28" s="10"/>
+      <c r="Y28" s="8"/>
       <c r="Z28" s="8"/>
       <c r="AA28" s="8">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AB28" s="10"/>
+      <c r="AB28" s="8"/>
       <c r="AC28" s="8"/>
       <c r="AD28" s="8">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AE28" s="10"/>
+      <c r="AE28" s="8"/>
       <c r="AF28" s="8"/>
       <c r="AG28" s="8">
         <f t="shared" si="58"/>
         <v>1</v>
       </c>
-      <c r="AH28" s="10"/>
+      <c r="AH28" s="8"/>
       <c r="AI28" s="8"/>
       <c r="AJ28" s="8">
         <f t="shared" si="59"/>
         <v>1</v>
       </c>
-      <c r="AK28" s="10"/>
+      <c r="AK28" s="8"/>
       <c r="AL28" s="8">
         <v>1</v>
       </c>
@@ -3646,37 +3643,37 @@
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="AN28" s="10"/>
+      <c r="AN28" s="8"/>
       <c r="AO28" s="8"/>
       <c r="AP28" s="8">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="AQ28" s="10"/>
+      <c r="AQ28" s="8"/>
       <c r="AR28" s="8"/>
       <c r="AS28" s="8">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
-      <c r="AT28" s="10"/>
+      <c r="AT28" s="8"/>
       <c r="AU28" s="8"/>
       <c r="AV28" s="8">
         <f t="shared" si="63"/>
         <v>0</v>
       </c>
-      <c r="AW28" s="10"/>
+      <c r="AW28" s="8"/>
       <c r="AX28" s="8"/>
       <c r="AY28" s="8">
         <f t="shared" si="64"/>
         <v>0</v>
       </c>
-      <c r="AZ28" s="11" t="e">
-        <f>H28+K28+N28+Q28+T28+W28+Z28+AC28+AF28+AI28+AL28+AO28+AR28+AU28+AX28+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA28" s="11" t="e">
+      <c r="AZ28" s="8">
+        <f>H28+K28+N28+Q28+T28+W28+Z28+AC28+AF28+AI28+AL28+AO28+AR28+AU28+AX28</f>
+        <v>1</v>
+      </c>
+      <c r="BA28" s="8">
         <f t="shared" si="65"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3699,61 +3696,61 @@
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
-      <c r="J29" s="10"/>
+      <c r="J29" s="8"/>
       <c r="K29" s="8"/>
       <c r="L29" s="8">
         <f t="shared" si="51"/>
         <v>1</v>
       </c>
-      <c r="M29" s="10"/>
+      <c r="M29" s="8"/>
       <c r="N29" s="8"/>
       <c r="O29" s="8">
         <f t="shared" si="52"/>
         <v>1</v>
       </c>
-      <c r="P29" s="10"/>
+      <c r="P29" s="8"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
-      <c r="S29" s="10"/>
+      <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8">
         <f t="shared" si="54"/>
         <v>1</v>
       </c>
-      <c r="V29" s="10"/>
+      <c r="V29" s="8"/>
       <c r="W29" s="8"/>
       <c r="X29" s="8">
         <f t="shared" si="55"/>
         <v>1</v>
       </c>
-      <c r="Y29" s="10"/>
+      <c r="Y29" s="8"/>
       <c r="Z29" s="8"/>
       <c r="AA29" s="8">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AB29" s="10"/>
+      <c r="AB29" s="8"/>
       <c r="AC29" s="8"/>
       <c r="AD29" s="8">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AE29" s="10"/>
+      <c r="AE29" s="8"/>
       <c r="AF29" s="8"/>
       <c r="AG29" s="8">
         <f t="shared" si="58"/>
         <v>1</v>
       </c>
-      <c r="AH29" s="10"/>
+      <c r="AH29" s="8"/>
       <c r="AI29" s="8"/>
       <c r="AJ29" s="8">
         <f t="shared" si="59"/>
         <v>1</v>
       </c>
-      <c r="AK29" s="10"/>
+      <c r="AK29" s="8"/>
       <c r="AL29" s="8">
         <v>1</v>
       </c>
@@ -3761,37 +3758,37 @@
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="AN29" s="10"/>
+      <c r="AN29" s="8"/>
       <c r="AO29" s="8"/>
       <c r="AP29" s="8">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="AQ29" s="10"/>
+      <c r="AQ29" s="8"/>
       <c r="AR29" s="8"/>
       <c r="AS29" s="8">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
-      <c r="AT29" s="10"/>
+      <c r="AT29" s="8"/>
       <c r="AU29" s="8"/>
       <c r="AV29" s="8">
         <f t="shared" si="63"/>
         <v>0</v>
       </c>
-      <c r="AW29" s="10"/>
+      <c r="AW29" s="8"/>
       <c r="AX29" s="8"/>
       <c r="AY29" s="8">
         <f t="shared" si="64"/>
         <v>0</v>
       </c>
-      <c r="AZ29" s="11" t="e">
-        <f>H29+K29+N29+Q29+T29+W29+Z29+AC29+AF29+AI29+AL29+AO29+AR29+AU29+AX29+#REF!+#REF!+#REF!+#REF!+#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="BA29" s="11" t="e">
+      <c r="AZ29" s="8">
+        <f>H29+K29+N29+Q29+T29+W29+Z29+AC29+AF29+AI29+AL29+AO29+AR29+AU29+AX29</f>
+        <v>1</v>
+      </c>
+      <c r="BA29" s="8">
         <f t="shared" si="65"/>
-        <v>#REF!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3804,7 +3801,7 @@
         <v>44</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="G30" s="5">
         <v>1</v>
@@ -3814,61 +3811,61 @@
         <f t="shared" si="50"/>
         <v>1</v>
       </c>
-      <c r="J30" s="10"/>
+      <c r="J30" s="8"/>
       <c r="K30" s="8"/>
       <c r="L30" s="8">
         <f t="shared" si="51"/>
         <v>1</v>
       </c>
-      <c r="M30" s="10"/>
+      <c r="M30" s="8"/>
       <c r="N30" s="8"/>
       <c r="O30" s="8">
         <f t="shared" si="52"/>
         <v>1</v>
       </c>
-      <c r="P30" s="10"/>
+      <c r="P30" s="8"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8">
         <f t="shared" si="53"/>
         <v>1</v>
       </c>
-      <c r="S30" s="10"/>
+      <c r="S30" s="8"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8">
         <f t="shared" si="54"/>
         <v>1</v>
       </c>
-      <c r="V30" s="10"/>
+      <c r="V30" s="8"/>
       <c r="W30" s="8"/>
       <c r="X30" s="8">
         <f t="shared" si="55"/>
         <v>1</v>
       </c>
-      <c r="Y30" s="10"/>
+      <c r="Y30" s="8"/>
       <c r="Z30" s="8"/>
       <c r="AA30" s="8">
         <f t="shared" si="56"/>
         <v>1</v>
       </c>
-      <c r="AB30" s="10"/>
+      <c r="AB30" s="8"/>
       <c r="AC30" s="8"/>
       <c r="AD30" s="8">
         <f t="shared" si="57"/>
         <v>1</v>
       </c>
-      <c r="AE30" s="10"/>
+      <c r="AE30" s="8"/>
       <c r="AF30" s="8"/>
       <c r="AG30" s="8">
         <f t="shared" si="58"/>
         <v>1</v>
       </c>
-      <c r="AH30" s="10"/>
+      <c r="AH30" s="8"/>
       <c r="AI30" s="8"/>
       <c r="AJ30" s="8">
         <f t="shared" si="59"/>
         <v>1</v>
       </c>
-      <c r="AK30" s="10"/>
+      <c r="AK30" s="8"/>
       <c r="AL30" s="8">
         <v>1</v>
       </c>
@@ -3876,41 +3873,276 @@
         <f t="shared" si="60"/>
         <v>0</v>
       </c>
-      <c r="AN30" s="10"/>
+      <c r="AN30" s="8"/>
       <c r="AO30" s="8"/>
       <c r="AP30" s="8">
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="AQ30" s="10"/>
+      <c r="AQ30" s="8"/>
       <c r="AR30" s="8"/>
       <c r="AS30" s="8">
         <f t="shared" si="62"/>
         <v>0</v>
       </c>
-      <c r="AT30" s="10"/>
+      <c r="AT30" s="8"/>
       <c r="AU30" s="8"/>
       <c r="AV30" s="8">
         <f t="shared" si="63"/>
         <v>0</v>
       </c>
-      <c r="AW30" s="10"/>
+      <c r="AW30" s="8"/>
       <c r="AX30" s="8"/>
       <c r="AY30" s="8">
         <f t="shared" si="64"/>
         <v>0</v>
       </c>
-      <c r="AZ30" s="11" t="e">
-        <f>H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30+#REF!+#REF!+#REF!+#REF!+#REF!</f>
+      <c r="AZ30" s="8">
+        <f>H30+K30+N30+Q30+T30+W30+Z30+AC30+AF30+AI30+AL30+AO30+AR30+AU30+AX30</f>
+        <v>1</v>
+      </c>
+      <c r="BA30" s="8">
+        <f t="shared" si="65"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="5">
+        <v>1</v>
+      </c>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8">
+        <f t="shared" ref="I31:I32" si="66">G31-H31</f>
+        <v>1</v>
+      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+      <c r="L31" s="8">
+        <f t="shared" ref="L31:L32" si="67">I31-K31</f>
+        <v>1</v>
+      </c>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8">
+        <f t="shared" ref="O31:O32" si="68">L31-N31</f>
+        <v>1</v>
+      </c>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8">
+        <f t="shared" ref="R31:R32" si="69">O31-Q31</f>
+        <v>1</v>
+      </c>
+      <c r="S31" s="8"/>
+      <c r="T31" s="8"/>
+      <c r="U31" s="8">
+        <f t="shared" ref="U31:U32" si="70">R31-T31</f>
+        <v>1</v>
+      </c>
+      <c r="V31" s="8"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="8">
+        <f t="shared" ref="X31:X32" si="71">U31-W31</f>
+        <v>1</v>
+      </c>
+      <c r="Y31" s="8"/>
+      <c r="Z31" s="8"/>
+      <c r="AA31" s="8">
+        <f t="shared" ref="AA31:AA32" si="72">X31-Z31</f>
+        <v>1</v>
+      </c>
+      <c r="AB31" s="8"/>
+      <c r="AC31" s="8"/>
+      <c r="AD31" s="8">
+        <f t="shared" ref="AD31:AD32" si="73">AA31-AC31</f>
+        <v>1</v>
+      </c>
+      <c r="AE31" s="8"/>
+      <c r="AF31" s="8"/>
+      <c r="AG31" s="8">
+        <f t="shared" ref="AG31:AG32" si="74">AD31-AF31</f>
+        <v>1</v>
+      </c>
+      <c r="AH31" s="8"/>
+      <c r="AI31" s="8"/>
+      <c r="AJ31" s="8">
+        <f t="shared" ref="AJ31:AJ32" si="75">AG31-AI31</f>
+        <v>1</v>
+      </c>
+      <c r="AK31" s="8"/>
+      <c r="AL31" s="8"/>
+      <c r="AM31" s="8">
+        <f t="shared" ref="AM31:AM32" si="76">AJ31-AL31</f>
+        <v>1</v>
+      </c>
+      <c r="AN31" s="8"/>
+      <c r="AO31" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP31" s="8">
+        <f t="shared" ref="AP31:AP32" si="77">AM31-AO31</f>
+        <v>0</v>
+      </c>
+      <c r="AQ31" s="8"/>
+      <c r="AR31" s="8"/>
+      <c r="AS31" s="8">
+        <f t="shared" ref="AS31:AS32" si="78">AP31-AR31</f>
+        <v>0</v>
+      </c>
+      <c r="AT31" s="8"/>
+      <c r="AU31" s="8"/>
+      <c r="AV31" s="8">
+        <f t="shared" ref="AV31:AV32" si="79">AS31-AU31</f>
+        <v>0</v>
+      </c>
+      <c r="AW31" s="8"/>
+      <c r="AX31" s="8"/>
+      <c r="AY31" s="8">
+        <f t="shared" ref="AY31:AY32" si="80">AV31-AX31</f>
+        <v>0</v>
+      </c>
+      <c r="AZ31" s="8">
+        <f>H31+K31+N31+Q31+T31+W31+Z31+AC31+AF31+AI31+AL31+AO31+AR31+AU31+AX31</f>
+        <v>1</v>
+      </c>
+      <c r="BA31" s="8">
+        <f t="shared" ref="BA31:BA32" si="81">G31-AZ31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:53" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="5">
+        <v>1</v>
+      </c>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8">
+        <f t="shared" si="66"/>
+        <v>1</v>
+      </c>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8">
+        <f t="shared" si="67"/>
+        <v>1</v>
+      </c>
+      <c r="M32" s="8"/>
+      <c r="N32" s="8"/>
+      <c r="O32" s="8">
+        <f t="shared" si="68"/>
+        <v>1</v>
+      </c>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="8"/>
+      <c r="R32" s="8">
+        <f t="shared" si="69"/>
+        <v>1</v>
+      </c>
+      <c r="S32" s="8"/>
+      <c r="T32" s="8"/>
+      <c r="U32" s="8">
+        <f t="shared" si="70"/>
+        <v>1</v>
+      </c>
+      <c r="V32" s="8"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="8">
+        <f t="shared" si="71"/>
+        <v>1</v>
+      </c>
+      <c r="Y32" s="8"/>
+      <c r="Z32" s="8"/>
+      <c r="AA32" s="8">
+        <f t="shared" si="72"/>
+        <v>1</v>
+      </c>
+      <c r="AB32" s="8"/>
+      <c r="AC32" s="8"/>
+      <c r="AD32" s="8">
+        <f t="shared" si="73"/>
+        <v>1</v>
+      </c>
+      <c r="AE32" s="8"/>
+      <c r="AF32" s="8"/>
+      <c r="AG32" s="8">
+        <f t="shared" si="74"/>
+        <v>1</v>
+      </c>
+      <c r="AH32" s="8"/>
+      <c r="AI32" s="8"/>
+      <c r="AJ32" s="8">
+        <f t="shared" si="75"/>
+        <v>1</v>
+      </c>
+      <c r="AK32" s="8"/>
+      <c r="AL32" s="8"/>
+      <c r="AM32" s="8">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="AN32" s="8"/>
+      <c r="AO32" s="8">
+        <v>1</v>
+      </c>
+      <c r="AP32" s="8">
+        <f t="shared" si="77"/>
+        <v>0</v>
+      </c>
+      <c r="AQ32" s="8"/>
+      <c r="AR32" s="8"/>
+      <c r="AS32" s="8">
+        <f t="shared" si="78"/>
+        <v>0</v>
+      </c>
+      <c r="AT32" s="8"/>
+      <c r="AU32" s="8"/>
+      <c r="AV32" s="8">
+        <f t="shared" si="79"/>
+        <v>0</v>
+      </c>
+      <c r="AW32" s="8"/>
+      <c r="AX32" s="8"/>
+      <c r="AY32" s="8">
+        <f t="shared" si="80"/>
+        <v>0</v>
+      </c>
+      <c r="AZ32" s="8" t="e">
+        <f>H32+K32+N32+Q32+T32+W32+Z32+AC32+AF32+AI32+AL32+AO32+AR32+AU32+AX32+#REF!+#REF!+#REF!+#REF!+#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="BA30" s="11" t="e">
-        <f t="shared" si="65"/>
+      <c r="BA32" s="8" t="e">
+        <f t="shared" si="81"/>
         <v>#REF!</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -3922,11 +4154,6 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>